<commit_message>
Create new data base for real use
</commit_message>
<xml_diff>
--- a/Document/ออกแบบDatabase.00.xlsx
+++ b/Document/ออกแบบDatabase.00.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Database\Oasis_Apartment_Program\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{6FCCAC7C-71C3-44FF-9A8C-A147A7E7C451}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E41D9BB-DB8B-4692-B5BD-9D4DFB8F24D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{2C372D90-7598-44C9-B553-6D996DEE060D}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{2C372D90-7598-44C9-B553-6D996DEE060D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -128,7 +128,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1334" uniqueCount="687">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1551" uniqueCount="753">
   <si>
     <t>ชื่อ</t>
   </si>
@@ -2333,6 +2333,204 @@
   </si>
   <si>
     <t>Access_Card_Manage_TBL</t>
+  </si>
+  <si>
+    <t>CREATE TABLE "Access_Card_Manage_TBL" (</t>
+  </si>
+  <si>
+    <t>INTEGER NOT NULL,</t>
+  </si>
+  <si>
+    <t>CardNo</t>
+  </si>
+  <si>
+    <t>TEXT,</t>
+  </si>
+  <si>
+    <t>INTEGER,</t>
+  </si>
+  <si>
+    <t>FOREIGN KEY("CustomerID") REFERENCES "Customer_TBL"("CustomerID"),</t>
+  </si>
+  <si>
+    <t>FOREIGN KEY("StaffID") REFERENCES "Employee_TBL"("EmployeeID"),</t>
+  </si>
+  <si>
+    <t>PRIMARY KEY("ID")</t>
+  </si>
+  <si>
+    <t>)</t>
+  </si>
+  <si>
+    <t>CREATE TABLE "Apartment_Info_TBL" (</t>
+  </si>
+  <si>
+    <t>RoomID    INTEGER NOT NULL,</t>
+  </si>
+  <si>
+    <t>RoomNo    TEXT NOT NULL UNIQUE,</t>
+  </si>
+  <si>
+    <t>Building    TEXT NOT NULL,</t>
+  </si>
+  <si>
+    <t>Floor    TEXT NOT NULL,</t>
+  </si>
+  <si>
+    <t>RoomType    TEXT NOT NULL,</t>
+  </si>
+  <si>
+    <t>PRIMARY KEY("RoomID" AUTOINCREMENT)</t>
+  </si>
+  <si>
+    <t>CREATE TABLE "Asset_TBL" (</t>
+  </si>
+  <si>
+    <t>Barcode    INTEGER NOT NULL UNIQUE,</t>
+  </si>
+  <si>
+    <t>Category    TEXT NOT NULL,</t>
+  </si>
+  <si>
+    <t>Item    TEXT NOT NULL,</t>
+  </si>
+  <si>
+    <t>PRIMARY KEY("Barcode" )</t>
+  </si>
+  <si>
+    <t>CREATE TABLE "Booking_TBL" (</t>
+  </si>
+  <si>
+    <t>BookingID</t>
+  </si>
+  <si>
+    <t>TEXT NOT NULL,</t>
+  </si>
+  <si>
+    <t>Remark</t>
+  </si>
+  <si>
+    <t>PRIMARY KEY("BookingID" AUTOINCREMENT),</t>
+  </si>
+  <si>
+    <t>FOREIGN KEY("RoomID") REFERENCES "Apartment_Info_TBL"("RoomID"),</t>
+  </si>
+  <si>
+    <t>FOREIGN KEY("CustomerID") REFERENCES "Customer_TBL"("CustomerID")</t>
+  </si>
+  <si>
+    <t>CREATE TABLE "Car_TBL" (</t>
+  </si>
+  <si>
+    <t>Brand_Model</t>
+  </si>
+  <si>
+    <t>TEXT NOT NULL UNIQUE,</t>
+  </si>
+  <si>
+    <t>DATE NOT NULL,</t>
+  </si>
+  <si>
+    <t>PRIMARY KEY("CarListID" AUTOINCREMENT),</t>
+  </si>
+  <si>
+    <t>CREATE TABLE "Contract_TBL" (</t>
+  </si>
+  <si>
+    <t>PRIMARY KEY("ContractID" AUTOINCREMENT),</t>
+  </si>
+  <si>
+    <t>CREATE TABLE "Customer_TBL" (</t>
+  </si>
+  <si>
+    <t>PRIMARY KEY("CustomerID" AUTOINCREMENT)</t>
+  </si>
+  <si>
+    <t>CREATE TABLE "Deposite_TBL" (</t>
+  </si>
+  <si>
+    <t>DepositeID    INTEGER NOT NULL,</t>
+  </si>
+  <si>
+    <t>Date    TEXT NOT NULL,</t>
+  </si>
+  <si>
+    <t>ItemBarcode    INTEGER NOT NULL,</t>
+  </si>
+  <si>
+    <t>Amount    INTEGER NOT NULL,</t>
+  </si>
+  <si>
+    <t>StaffID    INTEGER NOT NULL,</t>
+  </si>
+  <si>
+    <t>PRIMARY KEY("DepositeID" AUTOINCREMENT)</t>
+  </si>
+  <si>
+    <t>FOREIGN KEY("ItemBarcode") REFERENCES "Asset_TBL"("Barcode")</t>
+  </si>
+  <si>
+    <t>FOREIGN KEY("StaffID") REFERENCES "Employee_TBL"("EmployeeID")</t>
+  </si>
+  <si>
+    <t>CREATE TABLE "Employee_TBL" (</t>
+  </si>
+  <si>
+    <t>EmployeeID    INTEGER NOT NULL,</t>
+  </si>
+  <si>
+    <t>Prefix    TEXT NOT NULL,</t>
+  </si>
+  <si>
+    <t>FirstName    TEXT NOT NULL,</t>
+  </si>
+  <si>
+    <t>LastName    TEXT NOT NULL,</t>
+  </si>
+  <si>
+    <t>NickName    TEXT NOT NULL,</t>
+  </si>
+  <si>
+    <t>Phone    TEXT NOT NULL,</t>
+  </si>
+  <si>
+    <t>PRIMARY KEY("EmployeeID" AUTOINCREMENT)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>CREATE TABLE "Interested_People_TBL" (</t>
+  </si>
+  <si>
+    <t>PRIMARY KEY("InterestID" AUTOINCREMENT)</t>
+  </si>
+  <si>
+    <t>CREATE TABLE "Motocycle_TBL" (</t>
+  </si>
+  <si>
+    <t>MotocycleListID</t>
+  </si>
+  <si>
+    <t>PRIMARY KEY("MotocycleListID" AUTOINCREMENT)</t>
+  </si>
+  <si>
+    <t>CREATE TABLE "Withdraw_TBL" (</t>
+  </si>
+  <si>
+    <t>WithdrawID    INTEGER NOT NULL,</t>
+  </si>
+  <si>
+    <t>ItemBarcode    TEXT NOT NULL,</t>
+  </si>
+  <si>
+    <t>Withdrawer    INTEGER NOT NULL,</t>
+  </si>
+  <si>
+    <t>PRIMARY KEY("WithdrawID" AUTOINCREMENT)</t>
+  </si>
+  <si>
+    <t>FOREIGN KEY("Withdrawer") REFERENCES "Customer_TBL"("CustomerID")</t>
   </si>
 </sst>
 </file>
@@ -12253,12 +12451,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8947D8F6-B11D-4CEE-88B4-659BF9FBF640}">
-  <dimension ref="A1:AD593"/>
+  <dimension ref="A1:AG614"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane xSplit="13560" topLeftCell="U1"/>
-      <selection activeCell="G531" sqref="G531"/>
-      <selection pane="topRight" activeCell="U415" sqref="U415:V529"/>
+    <sheetView tabSelected="1" topLeftCell="A378" zoomScale="80" zoomScaleNormal="131" workbookViewId="0">
+      <pane xSplit="15444" topLeftCell="X1"/>
+      <selection activeCell="E391" sqref="E391"/>
+      <selection pane="topRight" activeCell="AE381" sqref="AE381:AE393"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -12320,6 +12518,9 @@
         <f>""""&amp;B3&amp;"""" &amp;"    "&amp; "INTEGER NOT NULL,"</f>
         <v>"EmployeeID"    INTEGER NOT NULL,</v>
       </c>
+      <c r="AB3" t="s">
+        <v>741</v>
+      </c>
     </row>
     <row r="4" spans="2:29" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B4" s="22"/>
@@ -12332,6 +12533,9 @@
         <f>""""&amp;C3&amp;"""" &amp;"    "&amp; "TEXT NOT NULL,"</f>
         <v>"Prefix"    TEXT NOT NULL,</v>
       </c>
+      <c r="AC4" t="s">
+        <v>734</v>
+      </c>
     </row>
     <row r="5" spans="2:29" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B5" s="22"/>
@@ -12344,6 +12548,9 @@
         <f>""""&amp;D3&amp;"""" &amp;"    "&amp; "TEXT NOT NULL,"</f>
         <v>"FirstName"    TEXT NOT NULL,</v>
       </c>
+      <c r="AC5" t="s">
+        <v>735</v>
+      </c>
     </row>
     <row r="6" spans="2:29" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B6" s="22"/>
@@ -12356,6 +12563,9 @@
         <f>""""&amp;E3&amp;"""" &amp;"    "&amp; "TEXT NOT NULL,"</f>
         <v>"LastName"    TEXT NOT NULL,</v>
       </c>
+      <c r="AC6" t="s">
+        <v>736</v>
+      </c>
     </row>
     <row r="7" spans="2:29" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B7" s="22"/>
@@ -12368,6 +12578,9 @@
         <f>""""&amp;F3&amp;"""" &amp;"    "&amp; "TEXT NOT NULL,"</f>
         <v>"NickName"    TEXT NOT NULL,</v>
       </c>
+      <c r="AC7" t="s">
+        <v>737</v>
+      </c>
     </row>
     <row r="8" spans="2:29" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B8" s="22"/>
@@ -12380,6 +12593,9 @@
         <f>""""&amp;G3&amp;"""" &amp;"    "&amp; "TEXT NOT NULL,"</f>
         <v>"Phone"    TEXT NOT NULL,</v>
       </c>
+      <c r="AC8" t="s">
+        <v>738</v>
+      </c>
     </row>
     <row r="9" spans="2:29" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B9" s="22"/>
@@ -12392,6 +12608,9 @@
         <f>"PRIMARY KEY("""&amp;  B3 &amp; """ AUTOINCREMENT)"</f>
         <v>PRIMARY KEY("EmployeeID" AUTOINCREMENT)</v>
       </c>
+      <c r="AC9" t="s">
+        <v>739</v>
+      </c>
     </row>
     <row r="10" spans="2:29" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B10" s="22"/>
@@ -12402,6 +12621,9 @@
       <c r="G10" s="23"/>
       <c r="V10" t="s">
         <v>518</v>
+      </c>
+      <c r="AC10" t="s">
+        <v>740</v>
       </c>
     </row>
     <row r="11" spans="2:29" ht="14.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
@@ -12415,6 +12637,9 @@
         <f>"INSERT INTO " &amp; B1 &amp; "(" &amp; C3 &amp;","&amp; D3 &amp;","&amp; E3 &amp;","&amp; F3 &amp;","&amp; G3 &amp; ")"</f>
         <v>INSERT INTO Employee_TBL(Prefix,FirstName,LastName,NickName,Phone)</v>
       </c>
+      <c r="AC11" t="s">
+        <v>695</v>
+      </c>
     </row>
     <row r="12" spans="2:29" x14ac:dyDescent="0.3">
       <c r="B12" s="7" t="s">
@@ -12442,6 +12667,9 @@
         <f t="shared" ref="V12:V22" si="0">"("&amp;FunNoo&amp;C12&amp;FunNooComma&amp;FunNoo&amp;D12&amp;FunNooComma&amp;FunNoo&amp;E12&amp;FunNooComma&amp;FunNoo&amp;F12&amp;FunNooComma&amp;FunNoo&amp;G12&amp;"""),"</f>
         <v>("นาย","ยศยุทธ","ดารกมาศ","โอ๊ต","084-1456263"),</v>
       </c>
+      <c r="AC12" t="s">
+        <v>733</v>
+      </c>
     </row>
     <row r="13" spans="2:29" x14ac:dyDescent="0.3">
       <c r="B13" s="7" t="s">
@@ -12490,6 +12718,9 @@
         <f t="shared" si="0"/>
         <v>("นาย","ประสิทธิ์","ใจแก้ว","แก้ว","081-793-9962"),</v>
       </c>
+      <c r="AC14" t="s">
+        <v>734</v>
+      </c>
     </row>
     <row r="15" spans="2:29" x14ac:dyDescent="0.3">
       <c r="B15" s="7" t="s">
@@ -12514,6 +12745,9 @@
         <f t="shared" si="0"/>
         <v>("นาง","อธิชา","ดารกมาศ","อ้อ","082-492-6956"),</v>
       </c>
+      <c r="AC15" t="s">
+        <v>735</v>
+      </c>
     </row>
     <row r="16" spans="2:29" x14ac:dyDescent="0.3">
       <c r="B16" s="7" t="s">
@@ -12538,8 +12772,11 @@
         <f t="shared" si="0"/>
         <v>("นาง","รัชนิกร","ดารกมาศ","จุก","082-486-5459"),</v>
       </c>
-    </row>
-    <row r="17" spans="2:22" x14ac:dyDescent="0.3">
+      <c r="AC16" t="s">
+        <v>736</v>
+      </c>
+    </row>
+    <row r="17" spans="2:29" x14ac:dyDescent="0.3">
       <c r="B17" s="7" t="s">
         <v>222</v>
       </c>
@@ -12562,8 +12799,11 @@
         <f t="shared" si="0"/>
         <v>("นางสาว","สิรภัทร","แสงกระจ่าง","แอม","084-699-7115"),</v>
       </c>
-    </row>
-    <row r="18" spans="2:22" x14ac:dyDescent="0.3">
+      <c r="AC17" t="s">
+        <v>737</v>
+      </c>
+    </row>
+    <row r="18" spans="2:29" x14ac:dyDescent="0.3">
       <c r="B18" s="7" t="s">
         <v>223</v>
       </c>
@@ -12586,8 +12826,11 @@
         <f t="shared" si="0"/>
         <v>("นาย","พงศนาถ","แสงกระจ่าง","อ๊อบ","082-394-9516"),</v>
       </c>
-    </row>
-    <row r="19" spans="2:22" x14ac:dyDescent="0.3">
+      <c r="AC18" t="s">
+        <v>738</v>
+      </c>
+    </row>
+    <row r="19" spans="2:29" x14ac:dyDescent="0.3">
       <c r="B19" s="7" t="s">
         <v>224</v>
       </c>
@@ -12610,8 +12853,11 @@
         <f t="shared" si="0"/>
         <v>("นางสาว","ใจดี","ดีใจ","จันจ้าว","089-998-8999"),</v>
       </c>
-    </row>
-    <row r="20" spans="2:22" x14ac:dyDescent="0.3">
+      <c r="AC19" t="s">
+        <v>739</v>
+      </c>
+    </row>
+    <row r="20" spans="2:29" x14ac:dyDescent="0.3">
       <c r="B20" s="7" t="s">
         <v>225</v>
       </c>
@@ -12634,8 +12880,11 @@
         <f t="shared" si="0"/>
         <v>("นางสาว","เอาใจ","ดูแล","อิงฟ้า","081-123-4567"),</v>
       </c>
-    </row>
-    <row r="21" spans="2:22" x14ac:dyDescent="0.3">
+      <c r="AC20" t="s">
+        <v>740</v>
+      </c>
+    </row>
+    <row r="21" spans="2:29" x14ac:dyDescent="0.3">
       <c r="B21" s="7" t="s">
         <v>226</v>
       </c>
@@ -12658,8 +12907,11 @@
         <f t="shared" si="0"/>
         <v>("นางสาว","ทุกระดับ","ประทับใจ","เม็ดทราย","087-767-7777"),</v>
       </c>
-    </row>
-    <row r="22" spans="2:22" x14ac:dyDescent="0.3">
+      <c r="AC21" t="s">
+        <v>695</v>
+      </c>
+    </row>
+    <row r="22" spans="2:29" x14ac:dyDescent="0.3">
       <c r="B22" s="7" t="s">
         <v>227</v>
       </c>
@@ -12683,7 +12935,7 @@
         <v>("นางสาว","ร่าเริง","แจ่มใส","น่านฟ้า","084-145-6789"),</v>
       </c>
     </row>
-    <row r="23" spans="2:22" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:29" x14ac:dyDescent="0.3">
       <c r="B23" s="7" t="s">
         <v>228</v>
       </c>
@@ -12707,28 +12959,28 @@
         <v>("นางสาว","ยินดี","ต้อนรับ","อั่งเปา","088-456-7898");</v>
       </c>
     </row>
-    <row r="24" spans="2:22" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:29" x14ac:dyDescent="0.3">
       <c r="B24" s="18"/>
       <c r="C24" s="8"/>
       <c r="D24" s="8"/>
       <c r="E24" s="8"/>
       <c r="F24" s="8"/>
     </row>
-    <row r="25" spans="2:22" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:29" x14ac:dyDescent="0.3">
       <c r="B25" s="18"/>
       <c r="C25" s="8"/>
       <c r="D25" s="8"/>
       <c r="E25" s="8"/>
       <c r="F25" s="8"/>
     </row>
-    <row r="26" spans="2:22" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:29" x14ac:dyDescent="0.3">
       <c r="B26" s="18"/>
       <c r="C26" s="8"/>
       <c r="D26" s="8"/>
       <c r="E26" s="8"/>
       <c r="F26" s="8"/>
     </row>
-    <row r="27" spans="2:22" ht="23.4" x14ac:dyDescent="0.45">
+    <row r="27" spans="2:29" ht="23.4" x14ac:dyDescent="0.45">
       <c r="B27" s="26" t="s">
         <v>421</v>
       </c>
@@ -12736,8 +12988,19 @@
         <f>"CREATE TABLE """ &amp;B27 &amp; """ ("</f>
         <v>CREATE TABLE "Customer_TBL" (</v>
       </c>
-    </row>
-    <row r="29" spans="2:22" ht="44.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="AA27" t="s">
+        <v>722</v>
+      </c>
+    </row>
+    <row r="28" spans="2:29" x14ac:dyDescent="0.3">
+      <c r="AB28" t="s">
+        <v>407</v>
+      </c>
+      <c r="AC28" t="s">
+        <v>688</v>
+      </c>
+    </row>
+    <row r="29" spans="2:29" ht="44.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B29" s="22" t="s">
         <v>407</v>
       </c>
@@ -12796,8 +13059,14 @@
         <f>""""&amp;B29&amp;"""" &amp;"    "&amp; "INTEGER NOT NULL,"</f>
         <v>"CustomerID"    INTEGER NOT NULL,</v>
       </c>
-    </row>
-    <row r="30" spans="2:22" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="AB29" t="s">
+        <v>401</v>
+      </c>
+      <c r="AC29" t="s">
+        <v>710</v>
+      </c>
+    </row>
+    <row r="30" spans="2:29" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B30" s="22"/>
       <c r="C30" s="23"/>
       <c r="D30" s="23"/>
@@ -12820,8 +13089,14 @@
         <f>""""&amp;C29&amp;"""" &amp;"    "&amp; "TEXT NOT NULL,"</f>
         <v>"Prefix"    TEXT NOT NULL,</v>
       </c>
-    </row>
-    <row r="31" spans="2:22" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="AB30" t="s">
+        <v>403</v>
+      </c>
+      <c r="AC30" t="s">
+        <v>710</v>
+      </c>
+    </row>
+    <row r="31" spans="2:29" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B31" s="22"/>
       <c r="C31" s="23"/>
       <c r="D31" s="23"/>
@@ -12844,8 +13119,14 @@
         <f>""""&amp;D29&amp;"""" &amp;"    "&amp; "TEXT NOT NULL,"</f>
         <v>"FirstName"    TEXT NOT NULL,</v>
       </c>
-    </row>
-    <row r="32" spans="2:22" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="AB31" t="s">
+        <v>404</v>
+      </c>
+      <c r="AC31" t="s">
+        <v>710</v>
+      </c>
+    </row>
+    <row r="32" spans="2:29" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B32" s="22"/>
       <c r="C32" s="23"/>
       <c r="D32" s="23"/>
@@ -12868,8 +13149,14 @@
         <f>""""&amp;E29&amp;"""" &amp;"    "&amp; "TEXT NOT NULL,"</f>
         <v>"LastName"    TEXT NOT NULL,</v>
       </c>
-    </row>
-    <row r="33" spans="2:22" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="AB32" t="s">
+        <v>405</v>
+      </c>
+      <c r="AC32" t="s">
+        <v>690</v>
+      </c>
+    </row>
+    <row r="33" spans="2:29" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B33" s="22"/>
       <c r="C33" s="23"/>
       <c r="D33" s="23"/>
@@ -12892,8 +13179,14 @@
         <f>""""&amp;F29&amp;"""" &amp;"    "&amp; "TEXT,"</f>
         <v>"NickName"    TEXT,</v>
       </c>
-    </row>
-    <row r="34" spans="2:22" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="AB33" t="s">
+        <v>408</v>
+      </c>
+      <c r="AC33" t="s">
+        <v>710</v>
+      </c>
+    </row>
+    <row r="34" spans="2:29" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B34" s="22"/>
       <c r="C34" s="23"/>
       <c r="D34" s="23"/>
@@ -12916,8 +13209,14 @@
         <f>""""&amp;G29&amp;"""" &amp;"    "&amp; "TEXT NOT NULL,"</f>
         <v>"ThaiNationalID"    TEXT NOT NULL,</v>
       </c>
-    </row>
-    <row r="35" spans="2:22" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="AB34" t="s">
+        <v>409</v>
+      </c>
+      <c r="AC34" t="s">
+        <v>710</v>
+      </c>
+    </row>
+    <row r="35" spans="2:29" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B35" s="22"/>
       <c r="C35" s="23"/>
       <c r="D35" s="23"/>
@@ -12940,8 +13239,14 @@
         <f>""""&amp;H29&amp;"""" &amp;"    "&amp; "TEXT NOT NULL,"</f>
         <v>"BirthDay"    TEXT NOT NULL,</v>
       </c>
-    </row>
-    <row r="36" spans="2:22" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="AB35" t="s">
+        <v>551</v>
+      </c>
+      <c r="AC35" t="s">
+        <v>690</v>
+      </c>
+    </row>
+    <row r="36" spans="2:29" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B36" s="22"/>
       <c r="C36" s="23"/>
       <c r="D36" s="23"/>
@@ -12964,8 +13269,14 @@
         <f>""""&amp;I29&amp;"""" &amp;"    "&amp; "TEXT NOT NULL,"</f>
         <v>"AddressNumber"    TEXT NOT NULL,</v>
       </c>
-    </row>
-    <row r="37" spans="2:22" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="AB36" t="s">
+        <v>517</v>
+      </c>
+      <c r="AC36" t="s">
+        <v>690</v>
+      </c>
+    </row>
+    <row r="37" spans="2:29" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B37" s="22"/>
       <c r="C37" s="23"/>
       <c r="D37" s="23"/>
@@ -12988,8 +13299,14 @@
         <f>""""&amp;J29&amp;"""" &amp;"    "&amp; "TEXT NOT NULL,"</f>
         <v>"AddressCont"    TEXT NOT NULL,</v>
       </c>
-    </row>
-    <row r="38" spans="2:22" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="AB37" t="s">
+        <v>493</v>
+      </c>
+      <c r="AC37" t="s">
+        <v>690</v>
+      </c>
+    </row>
+    <row r="38" spans="2:29" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B38" s="22"/>
       <c r="C38" s="23"/>
       <c r="D38" s="23"/>
@@ -13012,8 +13329,14 @@
         <f>""""&amp;K29&amp;"""" &amp;"    "&amp; "TEXT NOT NULL,"</f>
         <v>"AddressRoad"    TEXT NOT NULL,</v>
       </c>
-    </row>
-    <row r="39" spans="2:22" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="AB38" t="s">
+        <v>497</v>
+      </c>
+      <c r="AC38" t="s">
+        <v>690</v>
+      </c>
+    </row>
+    <row r="39" spans="2:29" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B39" s="22"/>
       <c r="C39" s="23"/>
       <c r="D39" s="23"/>
@@ -13036,8 +13359,14 @@
         <f>""""&amp;L29&amp;"""" &amp;"    "&amp; "TEXT NOT NULL,"</f>
         <v>"AddressSubProvince"    TEXT NOT NULL,</v>
       </c>
-    </row>
-    <row r="40" spans="2:22" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="AB39" t="s">
+        <v>496</v>
+      </c>
+      <c r="AC39" t="s">
+        <v>690</v>
+      </c>
+    </row>
+    <row r="40" spans="2:29" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B40" s="22"/>
       <c r="C40" s="23"/>
       <c r="D40" s="23"/>
@@ -13060,8 +13389,14 @@
         <f>""""&amp;M29&amp;"""" &amp;"    "&amp; "TEXT NOT NULL,"</f>
         <v>"AddressProvince"    TEXT NOT NULL,</v>
       </c>
-    </row>
-    <row r="41" spans="2:22" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="AB40" t="s">
+        <v>475</v>
+      </c>
+      <c r="AC40" t="s">
+        <v>690</v>
+      </c>
+    </row>
+    <row r="41" spans="2:29" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B41" s="22"/>
       <c r="C41" s="23"/>
       <c r="D41" s="23"/>
@@ -13084,8 +13419,14 @@
         <f>""""&amp;N29&amp;"""" &amp;"    "&amp; "TEXT NOT NULL,"</f>
         <v>"AddressCity"    TEXT NOT NULL,</v>
       </c>
-    </row>
-    <row r="42" spans="2:22" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="AB41" t="s">
+        <v>410</v>
+      </c>
+      <c r="AC41" t="s">
+        <v>690</v>
+      </c>
+    </row>
+    <row r="42" spans="2:29" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B42" s="22"/>
       <c r="C42" s="23"/>
       <c r="D42" s="23"/>
@@ -13108,8 +13449,14 @@
         <f>""""&amp;O29&amp;"""" &amp;"    "&amp; "TEXT NOT NULL,"</f>
         <v>"Phone"    TEXT NOT NULL,</v>
       </c>
-    </row>
-    <row r="43" spans="2:22" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="AB42" t="s">
+        <v>411</v>
+      </c>
+      <c r="AC42" t="s">
+        <v>690</v>
+      </c>
+    </row>
+    <row r="43" spans="2:29" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B43" s="22"/>
       <c r="C43" s="23"/>
       <c r="D43" s="23"/>
@@ -13132,8 +13479,14 @@
         <f>""""&amp;P29&amp;"""" &amp;"    "&amp; "TEXT,"</f>
         <v>"LineID"    TEXT,</v>
       </c>
-    </row>
-    <row r="44" spans="2:22" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="AB43" t="s">
+        <v>412</v>
+      </c>
+      <c r="AC43" t="s">
+        <v>690</v>
+      </c>
+    </row>
+    <row r="44" spans="2:29" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B44" s="22"/>
       <c r="C44" s="23"/>
       <c r="D44" s="23"/>
@@ -13156,8 +13509,14 @@
         <f>""""&amp;Q29&amp;"""" &amp;"    "&amp; "TEXT,"</f>
         <v>"Job"    TEXT,</v>
       </c>
-    </row>
-    <row r="45" spans="2:22" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="AB44" t="s">
+        <v>413</v>
+      </c>
+      <c r="AC44" t="s">
+        <v>690</v>
+      </c>
+    </row>
+    <row r="45" spans="2:29" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B45" s="22"/>
       <c r="C45" s="23"/>
       <c r="D45" s="23"/>
@@ -13180,8 +13539,14 @@
         <f>""""&amp;R29&amp;"""" &amp;"    "&amp; "TEXT,"</f>
         <v>"ReferencePerson"    TEXT,</v>
       </c>
-    </row>
-    <row r="46" spans="2:22" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="AB45" t="s">
+        <v>414</v>
+      </c>
+      <c r="AC45" t="s">
+        <v>710</v>
+      </c>
+    </row>
+    <row r="46" spans="2:29" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B46" s="22"/>
       <c r="C46" s="23"/>
       <c r="D46" s="23"/>
@@ -13204,8 +13569,11 @@
         <f>""""&amp;S29&amp;"""" &amp;"    "&amp; "TEXT NOT NULL,"</f>
         <v>"RegisterDate"    TEXT NOT NULL,</v>
       </c>
-    </row>
-    <row r="47" spans="2:22" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="AB46" t="s">
+        <v>723</v>
+      </c>
+    </row>
+    <row r="47" spans="2:29" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B47" s="22"/>
       <c r="C47" s="23"/>
       <c r="D47" s="23"/>
@@ -13228,8 +13596,11 @@
         <f>"PRIMARY KEY("""&amp;  B29 &amp; """ AUTOINCREMENT)"</f>
         <v>PRIMARY KEY("CustomerID" AUTOINCREMENT)</v>
       </c>
-    </row>
-    <row r="48" spans="2:22" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="AA47" t="s">
+        <v>695</v>
+      </c>
+    </row>
+    <row r="48" spans="2:29" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B48" s="22"/>
       <c r="C48" s="23"/>
       <c r="D48" s="23"/>
@@ -14864,7 +15235,7 @@
         <v>"MotorcycleListID"    INTEGER NOT NULL,</v>
       </c>
     </row>
-    <row r="81" spans="2:22" ht="34.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="81" spans="2:30" ht="34.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B81" s="24"/>
       <c r="C81" s="23"/>
       <c r="D81" s="23"/>
@@ -14876,7 +15247,7 @@
         <v>"Brand"    TEXT NOT NULL,</v>
       </c>
     </row>
-    <row r="82" spans="2:22" ht="34.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="82" spans="2:30" ht="34.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B82" s="24"/>
       <c r="C82" s="23"/>
       <c r="D82" s="23"/>
@@ -14888,7 +15259,7 @@
         <v>"Model"    TEXT NOT NULL,</v>
       </c>
     </row>
-    <row r="83" spans="2:22" ht="34.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="83" spans="2:30" ht="34.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B83" s="24"/>
       <c r="C83" s="23"/>
       <c r="D83" s="23"/>
@@ -14900,7 +15271,7 @@
         <v>"Color"    TEXT NOT NULL UNIQUE,</v>
       </c>
     </row>
-    <row r="84" spans="2:22" ht="34.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="84" spans="2:30" ht="34.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B84" s="24"/>
       <c r="C84" s="23"/>
       <c r="D84" s="23"/>
@@ -14912,7 +15283,7 @@
         <v>"PlateNo"    INTEGER NOT NULL,</v>
       </c>
     </row>
-    <row r="85" spans="2:22" ht="34.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="85" spans="2:30" ht="34.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B85" s="24"/>
       <c r="C85" s="23"/>
       <c r="D85" s="23"/>
@@ -14924,7 +15295,7 @@
         <v>"CustomerID"    TEXT NOT NULL,</v>
       </c>
     </row>
-    <row r="86" spans="2:22" ht="34.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="86" spans="2:30" ht="34.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B86" s="24"/>
       <c r="C86" s="23"/>
       <c r="D86" s="23"/>
@@ -14936,7 +15307,7 @@
         <v>PRIMARY KEY("MotorcycleListID" AUTOINCREMENT)</v>
       </c>
     </row>
-    <row r="87" spans="2:22" ht="34.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="87" spans="2:30" ht="34.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B87" s="24"/>
       <c r="C87" s="23"/>
       <c r="D87" s="23"/>
@@ -14948,7 +15319,7 @@
         <v>FOREIGN KEY("PlateNo") REFERENCES "Customer_TBL"("CustomerID")</v>
       </c>
     </row>
-    <row r="88" spans="2:22" ht="34.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="88" spans="2:30" ht="34.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B88" s="24"/>
       <c r="C88" s="23"/>
       <c r="D88" s="23"/>
@@ -14959,7 +15330,7 @@
         <v>518</v>
       </c>
     </row>
-    <row r="89" spans="2:22" ht="34.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="89" spans="2:30" ht="34.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B89" s="24"/>
       <c r="C89" s="23"/>
       <c r="D89" s="23"/>
@@ -14967,7 +15338,7 @@
       <c r="F89" s="23"/>
       <c r="G89" s="22"/>
     </row>
-    <row r="90" spans="2:22" x14ac:dyDescent="0.3">
+    <row r="90" spans="2:30" x14ac:dyDescent="0.3">
       <c r="B90" s="27">
         <v>1</v>
       </c>
@@ -14987,7 +15358,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="91" spans="2:22" x14ac:dyDescent="0.3">
+    <row r="91" spans="2:30" x14ac:dyDescent="0.3">
       <c r="B91" s="27">
         <v>2</v>
       </c>
@@ -15007,7 +15378,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="92" spans="2:22" x14ac:dyDescent="0.3">
+    <row r="92" spans="2:30" x14ac:dyDescent="0.3">
       <c r="B92" s="27">
         <v>3</v>
       </c>
@@ -15027,7 +15398,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="93" spans="2:22" x14ac:dyDescent="0.3">
+    <row r="93" spans="2:30" x14ac:dyDescent="0.3">
       <c r="B93" s="27">
         <v>4</v>
       </c>
@@ -15047,7 +15418,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="94" spans="2:22" x14ac:dyDescent="0.3">
+    <row r="94" spans="2:30" x14ac:dyDescent="0.3">
       <c r="B94" s="27">
         <v>5</v>
       </c>
@@ -15067,7 +15438,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="96" spans="2:22" ht="23.4" x14ac:dyDescent="0.45">
+    <row r="96" spans="2:30" ht="23.4" x14ac:dyDescent="0.45">
       <c r="B96" s="26" t="s">
         <v>629</v>
       </c>
@@ -15075,11 +15446,20 @@
         <f>"CREATE TABLE """ &amp;B96 &amp; """ ("</f>
         <v>CREATE TABLE "Car_TBL" (</v>
       </c>
-    </row>
-    <row r="97" spans="2:22" x14ac:dyDescent="0.3">
+      <c r="AD96" t="s">
+        <v>744</v>
+      </c>
+    </row>
+    <row r="97" spans="2:32" x14ac:dyDescent="0.3">
       <c r="B97" s="5"/>
-    </row>
-    <row r="98" spans="2:22" ht="34.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="AE97" t="s">
+        <v>745</v>
+      </c>
+      <c r="AF97" t="s">
+        <v>688</v>
+      </c>
+    </row>
+    <row r="98" spans="2:32" ht="34.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B98" s="24" t="s">
         <v>630</v>
       </c>
@@ -15102,8 +15482,14 @@
         <f>""""&amp;B98&amp;"""" &amp;"    "&amp; "INTEGER NOT NULL,"</f>
         <v>"CarListID"    INTEGER NOT NULL,</v>
       </c>
-    </row>
-    <row r="99" spans="2:22" ht="34.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="AE98" t="s">
+        <v>716</v>
+      </c>
+      <c r="AF98" t="s">
+        <v>710</v>
+      </c>
+    </row>
+    <row r="99" spans="2:32" ht="34.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B99" s="24"/>
       <c r="C99" s="23"/>
       <c r="D99" s="23"/>
@@ -15114,8 +15500,14 @@
         <f>""""&amp;C98&amp;"""" &amp;"    "&amp; "TEXT NOT NULL,"</f>
         <v>"Brand"    TEXT NOT NULL,</v>
       </c>
-    </row>
-    <row r="100" spans="2:22" ht="34.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="AE99" t="s">
+        <v>415</v>
+      </c>
+      <c r="AF99" t="s">
+        <v>710</v>
+      </c>
+    </row>
+    <row r="100" spans="2:32" ht="34.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B100" s="24"/>
       <c r="C100" s="23"/>
       <c r="D100" s="23"/>
@@ -15126,8 +15518,14 @@
         <f>""""&amp;D98&amp;"""" &amp;"    "&amp; "TEXT NOT NULL,"</f>
         <v>"Model"    TEXT NOT NULL,</v>
       </c>
-    </row>
-    <row r="101" spans="2:22" ht="34.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="AE100" t="s">
+        <v>616</v>
+      </c>
+      <c r="AF100" t="s">
+        <v>717</v>
+      </c>
+    </row>
+    <row r="101" spans="2:32" ht="34.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B101" s="24"/>
       <c r="C101" s="23"/>
       <c r="D101" s="23"/>
@@ -15138,8 +15536,14 @@
         <f>""""&amp;E98&amp;"""" &amp;"    "&amp; "TEXT NOT NULL UNIQUE,"</f>
         <v>"Color"    TEXT NOT NULL UNIQUE,</v>
       </c>
-    </row>
-    <row r="102" spans="2:22" ht="34.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="AE101" t="s">
+        <v>407</v>
+      </c>
+      <c r="AF101" t="s">
+        <v>688</v>
+      </c>
+    </row>
+    <row r="102" spans="2:32" ht="34.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B102" s="24"/>
       <c r="C102" s="23"/>
       <c r="D102" s="23"/>
@@ -15150,8 +15554,14 @@
         <f>""""&amp;F98&amp;"""" &amp;"    "&amp; "INTEGER NOT NULL,"</f>
         <v>"PlateNo"    INTEGER NOT NULL,</v>
       </c>
-    </row>
-    <row r="103" spans="2:22" ht="34.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="AE102" t="s">
+        <v>414</v>
+      </c>
+      <c r="AF102" t="s">
+        <v>718</v>
+      </c>
+    </row>
+    <row r="103" spans="2:32" ht="34.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B103" s="24"/>
       <c r="C103" s="23"/>
       <c r="D103" s="23"/>
@@ -15162,8 +15572,11 @@
         <f>""""&amp;G98&amp;"""" &amp;"    "&amp; "TEXT NOT NULL,"</f>
         <v>"CustomerID"    TEXT NOT NULL,</v>
       </c>
-    </row>
-    <row r="104" spans="2:22" ht="34.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="AE103" t="s">
+        <v>692</v>
+      </c>
+    </row>
+    <row r="104" spans="2:32" ht="34.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B104" s="24"/>
       <c r="C104" s="23"/>
       <c r="D104" s="23"/>
@@ -15174,8 +15587,11 @@
         <f>"PRIMARY KEY("""&amp;  B98 &amp; """ AUTOINCREMENT)"</f>
         <v>PRIMARY KEY("CarListID" AUTOINCREMENT)</v>
       </c>
-    </row>
-    <row r="105" spans="2:22" ht="34.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="AE104" t="s">
+        <v>746</v>
+      </c>
+    </row>
+    <row r="105" spans="2:32" ht="34.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B105" s="24"/>
       <c r="C105" s="23"/>
       <c r="D105" s="23"/>
@@ -15186,8 +15602,11 @@
         <f>"FOREIGN KEY("""&amp;F98&amp;""") " &amp; "REFERENCES """ &amp; B45&amp; """(""" &amp; B47 &amp;""")"</f>
         <v>FOREIGN KEY("PlateNo") REFERENCES ""("")</v>
       </c>
-    </row>
-    <row r="106" spans="2:22" ht="34.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="AD105" t="s">
+        <v>695</v>
+      </c>
+    </row>
+    <row r="106" spans="2:32" ht="34.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B106" s="24"/>
       <c r="C106" s="23"/>
       <c r="D106" s="23"/>
@@ -15198,7 +15617,7 @@
         <v>518</v>
       </c>
     </row>
-    <row r="107" spans="2:22" ht="34.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="107" spans="2:32" ht="34.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B107" s="24"/>
       <c r="C107" s="23"/>
       <c r="D107" s="23"/>
@@ -15206,7 +15625,7 @@
       <c r="F107" s="23"/>
       <c r="G107" s="22"/>
     </row>
-    <row r="108" spans="2:22" x14ac:dyDescent="0.3">
+    <row r="108" spans="2:32" x14ac:dyDescent="0.3">
       <c r="B108" s="27">
         <v>1</v>
       </c>
@@ -15226,7 +15645,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="109" spans="2:22" x14ac:dyDescent="0.3">
+    <row r="109" spans="2:32" x14ac:dyDescent="0.3">
       <c r="B109" s="27">
         <v>2</v>
       </c>
@@ -15246,7 +15665,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="110" spans="2:22" x14ac:dyDescent="0.3">
+    <row r="110" spans="2:32" x14ac:dyDescent="0.3">
       <c r="B110" s="27">
         <v>3</v>
       </c>
@@ -15266,7 +15685,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="111" spans="2:22" x14ac:dyDescent="0.3">
+    <row r="111" spans="2:32" x14ac:dyDescent="0.3">
       <c r="B111" s="27">
         <v>4</v>
       </c>
@@ -15286,7 +15705,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="112" spans="2:22" x14ac:dyDescent="0.3">
+    <row r="112" spans="2:32" x14ac:dyDescent="0.3">
       <c r="B112" s="27">
         <v>5</v>
       </c>
@@ -15306,7 +15725,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="113" spans="2:22" ht="23.4" x14ac:dyDescent="0.45">
+    <row r="113" spans="2:29" ht="23.4" x14ac:dyDescent="0.45">
       <c r="B113" s="26" t="s">
         <v>422</v>
       </c>
@@ -15314,11 +15733,14 @@
         <f>"CREATE TABLE """ &amp;B113 &amp; """ ("</f>
         <v>CREATE TABLE "Apartment_Info_TBL" (</v>
       </c>
-    </row>
-    <row r="114" spans="2:22" x14ac:dyDescent="0.3">
+      <c r="AC113" t="s">
+        <v>696</v>
+      </c>
+    </row>
+    <row r="114" spans="2:29" x14ac:dyDescent="0.3">
       <c r="B114" s="5"/>
     </row>
-    <row r="115" spans="2:22" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="115" spans="2:29" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B115" s="22" t="s">
         <v>417</v>
       </c>
@@ -15338,8 +15760,11 @@
         <f>""""&amp;B115&amp;"""" &amp;"    "&amp; "INTEGER NOT NULL,"</f>
         <v>"RoomID"    INTEGER NOT NULL,</v>
       </c>
-    </row>
-    <row r="116" spans="2:22" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="AC115" t="s">
+        <v>697</v>
+      </c>
+    </row>
+    <row r="116" spans="2:29" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B116" s="22"/>
       <c r="C116" s="23"/>
       <c r="D116" s="23"/>
@@ -15349,8 +15774,11 @@
         <f>""""&amp;C115&amp;"""" &amp;"    "&amp; "TEXT NOT NULL UNIQUE,"</f>
         <v>"RoomNo"    TEXT NOT NULL UNIQUE,</v>
       </c>
-    </row>
-    <row r="117" spans="2:22" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="AC116" t="s">
+        <v>698</v>
+      </c>
+    </row>
+    <row r="117" spans="2:29" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B117" s="22"/>
       <c r="C117" s="23"/>
       <c r="D117" s="23"/>
@@ -15360,8 +15788,11 @@
         <f>""""&amp;D115&amp;"""" &amp;"    "&amp; "TEXT NOT NULL,"</f>
         <v>"Building"    TEXT NOT NULL,</v>
       </c>
-    </row>
-    <row r="118" spans="2:22" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="AC117" t="s">
+        <v>699</v>
+      </c>
+    </row>
+    <row r="118" spans="2:29" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B118" s="22"/>
       <c r="C118" s="23"/>
       <c r="D118" s="23"/>
@@ -15371,8 +15802,11 @@
         <f>""""&amp;E115&amp;"""" &amp;"    "&amp; "TEXT NOT NULL,"</f>
         <v>"Floor"    TEXT NOT NULL,</v>
       </c>
-    </row>
-    <row r="119" spans="2:22" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="AC118" t="s">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="119" spans="2:29" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B119" s="22"/>
       <c r="C119" s="23"/>
       <c r="D119" s="23"/>
@@ -15382,8 +15816,11 @@
         <f>""""&amp;F115&amp;"""" &amp;"    "&amp; "TEXT NOT NULL,"</f>
         <v>"RoomType"    TEXT NOT NULL,</v>
       </c>
-    </row>
-    <row r="120" spans="2:22" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="AC119" t="s">
+        <v>701</v>
+      </c>
+    </row>
+    <row r="120" spans="2:29" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B120" s="22"/>
       <c r="C120" s="23"/>
       <c r="D120" s="23"/>
@@ -15393,8 +15830,11 @@
         <f>"PRIMARY KEY("""&amp;  B115 &amp; """ AUTOINCREMENT)"</f>
         <v>PRIMARY KEY("RoomID" AUTOINCREMENT)</v>
       </c>
-    </row>
-    <row r="121" spans="2:22" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="AC120" t="s">
+        <v>702</v>
+      </c>
+    </row>
+    <row r="121" spans="2:29" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B121" s="22"/>
       <c r="C121" s="23"/>
       <c r="D121" s="23"/>
@@ -15403,8 +15843,11 @@
       <c r="V121" t="s">
         <v>518</v>
       </c>
-    </row>
-    <row r="122" spans="2:22" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="AC121" t="s">
+        <v>695</v>
+      </c>
+    </row>
+    <row r="122" spans="2:29" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B122" s="22"/>
       <c r="C122" s="23"/>
       <c r="D122" s="23"/>
@@ -15415,7 +15858,7 @@
         <v>INSERT INTO Apartment_Info_TBL(RoomNo,Building,Floor,RoomType)</v>
       </c>
     </row>
-    <row r="123" spans="2:22" x14ac:dyDescent="0.3">
+    <row r="123" spans="2:29" x14ac:dyDescent="0.3">
       <c r="B123" s="28" t="s">
         <v>138</v>
       </c>
@@ -15439,7 +15882,7 @@
         <v>("A104","A","1","SmallType"),</v>
       </c>
     </row>
-    <row r="124" spans="2:22" x14ac:dyDescent="0.3">
+    <row r="124" spans="2:29" x14ac:dyDescent="0.3">
       <c r="B124" s="28" t="s">
         <v>139</v>
       </c>
@@ -15460,7 +15903,7 @@
         <v>("A105","A","1","SmallType"),</v>
       </c>
     </row>
-    <row r="125" spans="2:22" x14ac:dyDescent="0.3">
+    <row r="125" spans="2:29" x14ac:dyDescent="0.3">
       <c r="B125" s="28" t="s">
         <v>140</v>
       </c>
@@ -15481,7 +15924,7 @@
         <v>("A106","A","1","SmallType"),</v>
       </c>
     </row>
-    <row r="126" spans="2:22" x14ac:dyDescent="0.3">
+    <row r="126" spans="2:29" x14ac:dyDescent="0.3">
       <c r="B126" s="28" t="s">
         <v>141</v>
       </c>
@@ -15502,7 +15945,7 @@
         <v>("A107","A","1","SmallType"),</v>
       </c>
     </row>
-    <row r="127" spans="2:22" x14ac:dyDescent="0.3">
+    <row r="127" spans="2:29" x14ac:dyDescent="0.3">
       <c r="B127" s="28" t="s">
         <v>142</v>
       </c>
@@ -15523,7 +15966,7 @@
         <v>("A108","A","1","SmallType"),</v>
       </c>
     </row>
-    <row r="128" spans="2:22" x14ac:dyDescent="0.3">
+    <row r="128" spans="2:29" x14ac:dyDescent="0.3">
       <c r="B128" s="28" t="s">
         <v>143</v>
       </c>
@@ -16531,7 +16974,7 @@
         <v>("B310","B","3","BigType");</v>
       </c>
     </row>
-    <row r="177" spans="2:22" ht="23.4" x14ac:dyDescent="0.45">
+    <row r="177" spans="2:32" ht="23.4" x14ac:dyDescent="0.45">
       <c r="B177" s="26" t="s">
         <v>423</v>
       </c>
@@ -16540,7 +16983,7 @@
         <v>CREATE TABLE "Apartment_Price_TBL" (</v>
       </c>
     </row>
-    <row r="179" spans="2:22" ht="18" x14ac:dyDescent="0.3">
+    <row r="179" spans="2:32" ht="18" x14ac:dyDescent="0.3">
       <c r="B179" s="22" t="s">
         <v>424</v>
       </c>
@@ -16567,7 +17010,7 @@
         <v>"PriceID"    INTEGER NOT NULL,</v>
       </c>
     </row>
-    <row r="180" spans="2:22" ht="18" x14ac:dyDescent="0.3">
+    <row r="180" spans="2:32" ht="18" x14ac:dyDescent="0.3">
       <c r="B180" s="22"/>
       <c r="C180" s="23"/>
       <c r="D180" s="23"/>
@@ -16580,7 +17023,7 @@
         <v>"Date"    TEXT NOT NULL,</v>
       </c>
     </row>
-    <row r="181" spans="2:22" ht="18" x14ac:dyDescent="0.3">
+    <row r="181" spans="2:32" ht="18" x14ac:dyDescent="0.3">
       <c r="B181" s="22"/>
       <c r="C181" s="23"/>
       <c r="D181" s="23"/>
@@ -16593,7 +17036,7 @@
         <v>"SmallType"    INTEGER NOT NULL,</v>
       </c>
     </row>
-    <row r="182" spans="2:22" ht="18" x14ac:dyDescent="0.3">
+    <row r="182" spans="2:32" ht="18" x14ac:dyDescent="0.3">
       <c r="B182" s="22"/>
       <c r="C182" s="23"/>
       <c r="D182" s="23"/>
@@ -16606,7 +17049,7 @@
         <v>"BigType"    INTEGER NOT NULL,</v>
       </c>
     </row>
-    <row r="183" spans="2:22" ht="18" x14ac:dyDescent="0.3">
+    <row r="183" spans="2:32" ht="18" x14ac:dyDescent="0.3">
       <c r="B183" s="22"/>
       <c r="C183" s="23"/>
       <c r="D183" s="23"/>
@@ -16619,7 +17062,7 @@
         <v>"Internet"    INTEGER NOT NULL,</v>
       </c>
     </row>
-    <row r="184" spans="2:22" ht="18" x14ac:dyDescent="0.3">
+    <row r="184" spans="2:32" ht="18" x14ac:dyDescent="0.3">
       <c r="B184" s="22"/>
       <c r="C184" s="23"/>
       <c r="D184" s="23"/>
@@ -16632,7 +17075,7 @@
         <v>"Central"    INTEGER NOT NULL,</v>
       </c>
     </row>
-    <row r="185" spans="2:22" ht="18" x14ac:dyDescent="0.3">
+    <row r="185" spans="2:32" ht="18" x14ac:dyDescent="0.3">
       <c r="B185" s="22"/>
       <c r="C185" s="23"/>
       <c r="D185" s="23"/>
@@ -16645,7 +17088,7 @@
         <v>"Parking"    INTEGER NOT NULL,</v>
       </c>
     </row>
-    <row r="186" spans="2:22" ht="18" x14ac:dyDescent="0.3">
+    <row r="186" spans="2:32" ht="18" x14ac:dyDescent="0.3">
       <c r="B186" s="22"/>
       <c r="C186" s="23"/>
       <c r="D186" s="23"/>
@@ -16658,7 +17101,7 @@
         <v>PRIMARY KEY("PriceID" AUTOINCREMENT)</v>
       </c>
     </row>
-    <row r="187" spans="2:22" ht="18" x14ac:dyDescent="0.3">
+    <row r="187" spans="2:32" ht="18" x14ac:dyDescent="0.3">
       <c r="B187" s="22"/>
       <c r="C187" s="23"/>
       <c r="D187" s="23"/>
@@ -16670,7 +17113,7 @@
         <v>518</v>
       </c>
     </row>
-    <row r="188" spans="2:22" ht="18" x14ac:dyDescent="0.3">
+    <row r="188" spans="2:32" ht="18" x14ac:dyDescent="0.3">
       <c r="B188" s="22"/>
       <c r="C188" s="23"/>
       <c r="D188" s="23"/>
@@ -16679,7 +17122,7 @@
       <c r="G188" s="23"/>
       <c r="H188" s="23"/>
     </row>
-    <row r="189" spans="2:22" x14ac:dyDescent="0.3">
+    <row r="189" spans="2:32" x14ac:dyDescent="0.3">
       <c r="B189" s="28" t="s">
         <v>138</v>
       </c>
@@ -16702,7 +17145,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="191" spans="2:22" ht="23.4" x14ac:dyDescent="0.45">
+    <row r="191" spans="2:32" ht="23.4" x14ac:dyDescent="0.45">
       <c r="B191" s="26" t="s">
         <v>428</v>
       </c>
@@ -16710,11 +17153,20 @@
         <f>"CREATE TABLE """ &amp;B191 &amp; """ ("</f>
         <v>CREATE TABLE "Contract_TBL" (</v>
       </c>
-    </row>
-    <row r="192" spans="2:22" x14ac:dyDescent="0.3">
+      <c r="AD191" t="s">
+        <v>708</v>
+      </c>
+    </row>
+    <row r="192" spans="2:32" x14ac:dyDescent="0.3">
       <c r="B192" s="5"/>
-    </row>
-    <row r="193" spans="2:22" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="AE192" t="s">
+        <v>709</v>
+      </c>
+      <c r="AF192" t="s">
+        <v>688</v>
+      </c>
+    </row>
+    <row r="193" spans="2:32" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B193" s="22" t="s">
         <v>429</v>
       </c>
@@ -16755,8 +17207,14 @@
         <f>""""&amp;B193&amp;"""" &amp;"    "&amp; "INTEGER NOT NULL,"</f>
         <v>"ContractID"    INTEGER NOT NULL,</v>
       </c>
-    </row>
-    <row r="194" spans="2:22" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="AE193" t="s">
+        <v>417</v>
+      </c>
+      <c r="AF193" t="s">
+        <v>688</v>
+      </c>
+    </row>
+    <row r="194" spans="2:32" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B194" s="22"/>
       <c r="C194" s="22" t="s">
         <v>78</v>
@@ -16783,8 +17241,14 @@
         <f>""""&amp;C193&amp;"""" &amp;"    "&amp; "INTEGER NOT NULL,"</f>
         <v>"RoomID"    INTEGER NOT NULL,</v>
       </c>
-    </row>
-    <row r="195" spans="2:22" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="AE194" t="s">
+        <v>407</v>
+      </c>
+      <c r="AF194" t="s">
+        <v>688</v>
+      </c>
+    </row>
+    <row r="195" spans="2:32" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B195" s="22"/>
       <c r="C195" s="22" t="s">
         <v>84</v>
@@ -16812,8 +17276,14 @@
         <f>""""&amp;D193&amp;"""" &amp;"    "&amp; "INTEGER NOT NULL,"</f>
         <v>"CustomerID"    INTEGER NOT NULL,</v>
       </c>
-    </row>
-    <row r="196" spans="2:22" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="AE195" t="s">
+        <v>430</v>
+      </c>
+      <c r="AF195" t="s">
+        <v>710</v>
+      </c>
+    </row>
+    <row r="196" spans="2:32" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B196" s="22"/>
       <c r="C196" s="22"/>
       <c r="D196" s="22"/>
@@ -16830,8 +17300,14 @@
         <f>""""&amp;E193&amp;"""" &amp;"    "&amp; "TEXT NOT NULL,"</f>
         <v>"CarPlateNo"    TEXT NOT NULL,</v>
       </c>
-    </row>
-    <row r="197" spans="2:22" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="AE196" t="s">
+        <v>431</v>
+      </c>
+      <c r="AF196" t="s">
+        <v>710</v>
+      </c>
+    </row>
+    <row r="197" spans="2:32" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B197" s="22"/>
       <c r="C197" s="22"/>
       <c r="D197" s="22"/>
@@ -16848,8 +17324,14 @@
         <f>""""&amp;F193&amp;"""" &amp;"    "&amp; "TEXT NOT NULL,"</f>
         <v>"StartDate"    TEXT NOT NULL,</v>
       </c>
-    </row>
-    <row r="198" spans="2:22" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="AE197" t="s">
+        <v>522</v>
+      </c>
+      <c r="AF197" t="s">
+        <v>688</v>
+      </c>
+    </row>
+    <row r="198" spans="2:32" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B198" s="22"/>
       <c r="C198" s="22"/>
       <c r="D198" s="22"/>
@@ -16866,8 +17348,14 @@
         <f>""""&amp;G193&amp;"""" &amp;"    "&amp; "INTEGER NOT NULL,"</f>
         <v>"EndDate"    INTEGER NOT NULL,</v>
       </c>
-    </row>
-    <row r="199" spans="2:22" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="AE198" t="s">
+        <v>579</v>
+      </c>
+      <c r="AF198" t="s">
+        <v>688</v>
+      </c>
+    </row>
+    <row r="199" spans="2:32" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B199" s="22"/>
       <c r="C199" s="22"/>
       <c r="D199" s="22"/>
@@ -16884,8 +17372,14 @@
         <f>""""&amp;H193&amp;"""" &amp;"    "&amp; "TEXT NOT NULL,"</f>
         <v>"StaffID"    TEXT NOT NULL,</v>
       </c>
-    </row>
-    <row r="200" spans="2:22" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="AE199" t="s">
+        <v>578</v>
+      </c>
+      <c r="AF199" t="s">
+        <v>688</v>
+      </c>
+    </row>
+    <row r="200" spans="2:32" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B200" s="22"/>
       <c r="C200" s="22"/>
       <c r="D200" s="22"/>
@@ -16902,8 +17396,14 @@
         <f>"PRIMARY KEY("""&amp;  B193 &amp; """ AUTOINCREMENT)"</f>
         <v>PRIMARY KEY("ContractID" AUTOINCREMENT)</v>
       </c>
-    </row>
-    <row r="201" spans="2:22" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="AE200" t="s">
+        <v>584</v>
+      </c>
+      <c r="AF200" t="s">
+        <v>688</v>
+      </c>
+    </row>
+    <row r="201" spans="2:32" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B201" s="22"/>
       <c r="C201" s="22"/>
       <c r="D201" s="22"/>
@@ -16920,8 +17420,14 @@
         <f>"FOREIGN KEY("""&amp;C193&amp;""") " &amp; "REFERENCES """ &amp;B113&amp; """(""" &amp; B115 &amp;""")"</f>
         <v>FOREIGN KEY("RoomID") REFERENCES "Apartment_Info_TBL"("RoomID")</v>
       </c>
-    </row>
-    <row r="202" spans="2:22" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="AE201" t="s">
+        <v>580</v>
+      </c>
+      <c r="AF201" t="s">
+        <v>688</v>
+      </c>
+    </row>
+    <row r="202" spans="2:32" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B202" s="22"/>
       <c r="C202" s="22"/>
       <c r="D202" s="22"/>
@@ -16938,8 +17444,14 @@
         <f>"FOREIGN KEY("""&amp;D193&amp;""") " &amp; "REFERENCES """ &amp; B27&amp; """(""" &amp; B29 &amp;""")"</f>
         <v>FOREIGN KEY("CustomerID") REFERENCES "Customer_TBL"("CustomerID")</v>
       </c>
-    </row>
-    <row r="203" spans="2:22" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="AE202" t="s">
+        <v>711</v>
+      </c>
+      <c r="AF202" t="s">
+        <v>690</v>
+      </c>
+    </row>
+    <row r="203" spans="2:32" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B203" s="22"/>
       <c r="C203" s="22"/>
       <c r="D203" s="22"/>
@@ -16956,8 +17468,14 @@
         <f>"FOREIGN KEY("""&amp;G193&amp;""") " &amp; "REFERENCES """ &amp; B1&amp; """(""" &amp; B3 &amp;""")"</f>
         <v>FOREIGN KEY("EndDate") REFERENCES "Employee_TBL"("EmployeeID")</v>
       </c>
-    </row>
-    <row r="204" spans="2:22" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="AE203" t="s">
+        <v>416</v>
+      </c>
+      <c r="AF203" t="s">
+        <v>710</v>
+      </c>
+    </row>
+    <row r="204" spans="2:32" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B204" s="22"/>
       <c r="C204" s="22"/>
       <c r="D204" s="22"/>
@@ -16973,8 +17491,11 @@
       <c r="V204" t="s">
         <v>518</v>
       </c>
-    </row>
-    <row r="205" spans="2:22" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="AE204" t="s">
+        <v>712</v>
+      </c>
+    </row>
+    <row r="205" spans="2:32" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B205" s="22"/>
       <c r="C205" s="22"/>
       <c r="D205" s="22"/>
@@ -16987,8 +17508,11 @@
       <c r="K205" s="25"/>
       <c r="L205" s="25"/>
       <c r="M205" s="25"/>
-    </row>
-    <row r="206" spans="2:22" x14ac:dyDescent="0.3">
+      <c r="AE205" t="s">
+        <v>693</v>
+      </c>
+    </row>
+    <row r="206" spans="2:32" x14ac:dyDescent="0.3">
       <c r="B206" s="7"/>
       <c r="C206" s="9"/>
       <c r="D206" s="7"/>
@@ -17001,8 +17525,11 @@
       <c r="K206" s="21"/>
       <c r="L206" s="21"/>
       <c r="M206" s="21"/>
-    </row>
-    <row r="207" spans="2:22" x14ac:dyDescent="0.3">
+      <c r="AE206" t="s">
+        <v>713</v>
+      </c>
+    </row>
+    <row r="207" spans="2:32" x14ac:dyDescent="0.3">
       <c r="B207" s="7"/>
       <c r="C207" s="9"/>
       <c r="D207" s="7"/>
@@ -17015,8 +17542,14 @@
       <c r="K207" s="1"/>
       <c r="L207" s="1"/>
       <c r="M207" s="1"/>
-    </row>
-    <row r="208" spans="2:22" x14ac:dyDescent="0.3">
+      <c r="V207" t="s">
+        <v>720</v>
+      </c>
+      <c r="AE207" t="s">
+        <v>714</v>
+      </c>
+    </row>
+    <row r="208" spans="2:32" x14ac:dyDescent="0.3">
       <c r="B208" s="7"/>
       <c r="C208" s="9"/>
       <c r="D208" s="7"/>
@@ -17029,8 +17562,17 @@
       <c r="K208" s="1"/>
       <c r="L208" s="1"/>
       <c r="M208" s="1"/>
-    </row>
-    <row r="209" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="W208" t="s">
+        <v>429</v>
+      </c>
+      <c r="X208" t="s">
+        <v>688</v>
+      </c>
+      <c r="AD208" t="s">
+        <v>695</v>
+      </c>
+    </row>
+    <row r="209" spans="2:24" x14ac:dyDescent="0.3">
       <c r="B209" s="7"/>
       <c r="C209" s="9"/>
       <c r="D209" s="7"/>
@@ -17043,8 +17585,14 @@
       <c r="K209" s="1"/>
       <c r="L209" s="1"/>
       <c r="M209" s="1"/>
-    </row>
-    <row r="210" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="W209" t="s">
+        <v>417</v>
+      </c>
+      <c r="X209" t="s">
+        <v>688</v>
+      </c>
+    </row>
+    <row r="210" spans="2:24" x14ac:dyDescent="0.3">
       <c r="B210" s="7"/>
       <c r="C210" s="9"/>
       <c r="D210" s="7"/>
@@ -17057,8 +17605,14 @@
       <c r="K210" s="1"/>
       <c r="L210" s="1"/>
       <c r="M210" s="1"/>
-    </row>
-    <row r="211" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="W210" t="s">
+        <v>407</v>
+      </c>
+      <c r="X210" t="s">
+        <v>688</v>
+      </c>
+    </row>
+    <row r="211" spans="2:24" x14ac:dyDescent="0.3">
       <c r="B211" s="7"/>
       <c r="C211" s="9"/>
       <c r="D211" s="7"/>
@@ -17071,8 +17625,14 @@
       <c r="K211" s="1"/>
       <c r="L211" s="1"/>
       <c r="M211" s="1"/>
-    </row>
-    <row r="212" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="W211" t="s">
+        <v>430</v>
+      </c>
+      <c r="X211" t="s">
+        <v>710</v>
+      </c>
+    </row>
+    <row r="212" spans="2:24" x14ac:dyDescent="0.3">
       <c r="B212" s="7"/>
       <c r="C212" s="9"/>
       <c r="D212" s="7"/>
@@ -17085,8 +17645,14 @@
       <c r="K212" s="1"/>
       <c r="L212" s="1"/>
       <c r="M212" s="1"/>
-    </row>
-    <row r="213" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="W212" t="s">
+        <v>431</v>
+      </c>
+      <c r="X212" t="s">
+        <v>710</v>
+      </c>
+    </row>
+    <row r="213" spans="2:24" x14ac:dyDescent="0.3">
       <c r="B213" s="7"/>
       <c r="C213" s="9"/>
       <c r="D213" s="7"/>
@@ -17099,8 +17665,14 @@
       <c r="K213" s="1"/>
       <c r="L213" s="1"/>
       <c r="M213" s="1"/>
-    </row>
-    <row r="214" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="W213" t="s">
+        <v>522</v>
+      </c>
+      <c r="X213" t="s">
+        <v>688</v>
+      </c>
+    </row>
+    <row r="214" spans="2:24" x14ac:dyDescent="0.3">
       <c r="B214" s="7"/>
       <c r="C214" s="9"/>
       <c r="D214" s="7"/>
@@ -17113,8 +17685,14 @@
       <c r="K214" s="1"/>
       <c r="L214" s="1"/>
       <c r="M214" s="1"/>
-    </row>
-    <row r="215" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="W214" t="s">
+        <v>579</v>
+      </c>
+      <c r="X214" t="s">
+        <v>688</v>
+      </c>
+    </row>
+    <row r="215" spans="2:24" x14ac:dyDescent="0.3">
       <c r="B215" s="7"/>
       <c r="C215" s="9"/>
       <c r="D215" s="7"/>
@@ -17127,8 +17705,14 @@
       <c r="K215" s="1"/>
       <c r="L215" s="1"/>
       <c r="M215" s="1"/>
-    </row>
-    <row r="216" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="W215" t="s">
+        <v>578</v>
+      </c>
+      <c r="X215" t="s">
+        <v>688</v>
+      </c>
+    </row>
+    <row r="216" spans="2:24" x14ac:dyDescent="0.3">
       <c r="B216" s="7"/>
       <c r="C216" s="9"/>
       <c r="D216" s="7"/>
@@ -17141,8 +17725,14 @@
       <c r="K216" s="1"/>
       <c r="L216" s="1"/>
       <c r="M216" s="1"/>
-    </row>
-    <row r="217" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="W216" t="s">
+        <v>584</v>
+      </c>
+      <c r="X216" t="s">
+        <v>688</v>
+      </c>
+    </row>
+    <row r="217" spans="2:24" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B217" s="14"/>
       <c r="C217" s="17"/>
       <c r="D217" s="14"/>
@@ -17155,8 +17745,14 @@
       <c r="K217" s="15"/>
       <c r="L217" s="15"/>
       <c r="M217" s="15"/>
-    </row>
-    <row r="218" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="W217" t="s">
+        <v>580</v>
+      </c>
+      <c r="X217" t="s">
+        <v>688</v>
+      </c>
+    </row>
+    <row r="218" spans="2:24" x14ac:dyDescent="0.3">
       <c r="B218" s="13"/>
       <c r="C218" s="16"/>
       <c r="D218" s="13"/>
@@ -17169,8 +17765,14 @@
       <c r="K218" s="21"/>
       <c r="L218" s="21"/>
       <c r="M218" s="21"/>
-    </row>
-    <row r="219" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="W218" t="s">
+        <v>711</v>
+      </c>
+      <c r="X218" t="s">
+        <v>690</v>
+      </c>
+    </row>
+    <row r="219" spans="2:24" x14ac:dyDescent="0.3">
       <c r="B219" s="7"/>
       <c r="C219" s="9"/>
       <c r="D219" s="7"/>
@@ -17183,8 +17785,14 @@
       <c r="K219" s="1"/>
       <c r="L219" s="1"/>
       <c r="M219" s="1"/>
-    </row>
-    <row r="220" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="W219" t="s">
+        <v>416</v>
+      </c>
+      <c r="X219" t="s">
+        <v>710</v>
+      </c>
+    </row>
+    <row r="220" spans="2:24" x14ac:dyDescent="0.3">
       <c r="B220" s="7"/>
       <c r="C220" s="9"/>
       <c r="D220" s="7"/>
@@ -17197,8 +17805,11 @@
       <c r="K220" s="1"/>
       <c r="L220" s="1"/>
       <c r="M220" s="1"/>
-    </row>
-    <row r="221" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="W220" t="s">
+        <v>721</v>
+      </c>
+    </row>
+    <row r="221" spans="2:24" x14ac:dyDescent="0.3">
       <c r="B221" s="7"/>
       <c r="C221" s="9"/>
       <c r="D221" s="7"/>
@@ -17211,8 +17822,11 @@
       <c r="K221" s="1"/>
       <c r="L221" s="1"/>
       <c r="M221" s="1"/>
-    </row>
-    <row r="222" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="W221" t="s">
+        <v>693</v>
+      </c>
+    </row>
+    <row r="222" spans="2:24" x14ac:dyDescent="0.3">
       <c r="B222" s="7"/>
       <c r="C222" s="9"/>
       <c r="D222" s="7"/>
@@ -17225,8 +17839,11 @@
       <c r="K222" s="1"/>
       <c r="L222" s="1"/>
       <c r="M222" s="1"/>
-    </row>
-    <row r="223" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="W222" t="s">
+        <v>713</v>
+      </c>
+    </row>
+    <row r="223" spans="2:24" x14ac:dyDescent="0.3">
       <c r="B223" s="7"/>
       <c r="C223" s="9"/>
       <c r="D223" s="7"/>
@@ -17239,8 +17856,11 @@
       <c r="K223" s="1"/>
       <c r="L223" s="1"/>
       <c r="M223" s="1"/>
-    </row>
-    <row r="224" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="W223" t="s">
+        <v>714</v>
+      </c>
+    </row>
+    <row r="224" spans="2:24" x14ac:dyDescent="0.3">
       <c r="B224" s="7"/>
       <c r="C224" s="9"/>
       <c r="D224" s="7"/>
@@ -17253,6 +17873,9 @@
       <c r="K224" s="1"/>
       <c r="L224" s="1"/>
       <c r="M224" s="1"/>
+      <c r="V224" t="s">
+        <v>695</v>
+      </c>
     </row>
     <row r="225" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B225" s="7"/>
@@ -18769,7 +19392,7 @@
       <c r="L304" s="33"/>
       <c r="M304" s="33"/>
     </row>
-    <row r="305" spans="2:22" ht="23.4" x14ac:dyDescent="0.45">
+    <row r="305" spans="2:29" ht="23.4" x14ac:dyDescent="0.45">
       <c r="B305" s="26" t="s">
         <v>437</v>
       </c>
@@ -18789,8 +19412,11 @@
         <f>"CREATE TABLE """ &amp;B305 &amp; """ ("</f>
         <v>CREATE TABLE "Asset_TBL" (</v>
       </c>
-    </row>
-    <row r="306" spans="2:22" x14ac:dyDescent="0.3">
+      <c r="AC305" t="s">
+        <v>703</v>
+      </c>
+    </row>
+    <row r="306" spans="2:29" x14ac:dyDescent="0.3">
       <c r="B306" s="5"/>
       <c r="D306" t="s">
         <v>524</v>
@@ -18805,7 +19431,7 @@
         <v>527</v>
       </c>
     </row>
-    <row r="307" spans="2:22" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="307" spans="2:29" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B307" s="22" t="s">
         <v>1</v>
       </c>
@@ -18822,8 +19448,11 @@
         <f>""""&amp;B307&amp;"""" &amp;"    "&amp; "INTEGER NOT NULL UNIQUE,"</f>
         <v>"Barcode"    INTEGER NOT NULL UNIQUE,</v>
       </c>
-    </row>
-    <row r="308" spans="2:22" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="AC307" t="s">
+        <v>704</v>
+      </c>
+    </row>
+    <row r="308" spans="2:29" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B308" s="22"/>
       <c r="C308" s="23"/>
       <c r="D308" s="23"/>
@@ -18834,8 +19463,11 @@
         <f>""""&amp;C307&amp;"""" &amp;"    "&amp; "TEXT NOT NULL,"</f>
         <v>"Category"    TEXT NOT NULL,</v>
       </c>
-    </row>
-    <row r="309" spans="2:22" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="AC308" t="s">
+        <v>705</v>
+      </c>
+    </row>
+    <row r="309" spans="2:29" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B309" s="22"/>
       <c r="C309" s="23"/>
       <c r="D309" s="23"/>
@@ -18846,8 +19478,11 @@
         <f>""""&amp;D307&amp;"""" &amp;"    "&amp; "TEXT NOT NULL,"</f>
         <v>"Item"    TEXT NOT NULL,</v>
       </c>
-    </row>
-    <row r="310" spans="2:22" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="AC309" t="s">
+        <v>706</v>
+      </c>
+    </row>
+    <row r="310" spans="2:29" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B310" s="22"/>
       <c r="C310" s="23"/>
       <c r="D310" s="23"/>
@@ -18858,16 +19493,22 @@
         <f>"PRIMARY KEY("""&amp;  B307 &amp; """ )"</f>
         <v>PRIMARY KEY("Barcode" )</v>
       </c>
-    </row>
-    <row r="311" spans="2:22" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="AC310" t="s">
+        <v>707</v>
+      </c>
+    </row>
+    <row r="311" spans="2:29" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B311" s="22"/>
       <c r="C311" s="23"/>
       <c r="D311" s="23"/>
       <c r="V311" t="s">
         <v>518</v>
       </c>
-    </row>
-    <row r="312" spans="2:22" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="AC311" t="s">
+        <v>695</v>
+      </c>
+    </row>
+    <row r="312" spans="2:29" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B312" s="22"/>
       <c r="C312" s="23"/>
       <c r="D312" s="23"/>
@@ -18876,7 +19517,7 @@
         <v>INSERT INTO Asset_TBL(Barcode,Category,Item)</v>
       </c>
     </row>
-    <row r="313" spans="2:22" x14ac:dyDescent="0.3">
+    <row r="313" spans="2:29" x14ac:dyDescent="0.3">
       <c r="B313" s="31" t="str">
         <f>$D$305&amp;$E$305&amp;"0000"&amp;$G$305</f>
         <v>885000000002</v>
@@ -18895,7 +19536,7 @@
         <v>("885000000002","ความปลอดภัย","Access Card"),</v>
       </c>
     </row>
-    <row r="314" spans="2:22" x14ac:dyDescent="0.3">
+    <row r="314" spans="2:29" x14ac:dyDescent="0.3">
       <c r="B314" s="31" t="str">
         <f>$D$305&amp;$E$305&amp;"0001"&amp;$G$305</f>
         <v>885000000012</v>
@@ -18911,12 +19552,12 @@
         <v>("885000000012","ความปลอดภัย","กุญแจห้อง"),</v>
       </c>
     </row>
-    <row r="315" spans="2:22" x14ac:dyDescent="0.3">
+    <row r="315" spans="2:29" x14ac:dyDescent="0.3">
       <c r="B315" s="1"/>
       <c r="C315" s="1"/>
       <c r="D315" s="1"/>
     </row>
-    <row r="316" spans="2:22" x14ac:dyDescent="0.3">
+    <row r="316" spans="2:29" x14ac:dyDescent="0.3">
       <c r="B316" s="1" t="str">
         <f>$D$305&amp;$E$305&amp;"1000"&amp;$G$305</f>
         <v>885000010002</v>
@@ -18932,7 +19573,7 @@
         <v>("885000010002","ไฟฟ้า","หลอดไฟห้อง"),</v>
       </c>
     </row>
-    <row r="317" spans="2:22" x14ac:dyDescent="0.3">
+    <row r="317" spans="2:29" x14ac:dyDescent="0.3">
       <c r="B317" s="1" t="str">
         <f>$D$305&amp;$E$305&amp;"1001"&amp;$G$305</f>
         <v>885000010012</v>
@@ -18948,7 +19589,7 @@
         <v>("885000010012","ไฟฟ้า","หลอดไฟห้องน้ำ"),</v>
       </c>
     </row>
-    <row r="318" spans="2:22" x14ac:dyDescent="0.3">
+    <row r="318" spans="2:29" x14ac:dyDescent="0.3">
       <c r="B318" s="1" t="str">
         <f>$D$305&amp;$E$305&amp;"1002"&amp;$G$305</f>
         <v>885000010022</v>
@@ -18964,12 +19605,12 @@
         <v>("885000010022","ไฟฟ้า","หลอดไฟระเบียง"),</v>
       </c>
     </row>
-    <row r="319" spans="2:22" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="319" spans="2:29" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B319" s="36"/>
       <c r="C319" s="36"/>
       <c r="D319" s="36"/>
     </row>
-    <row r="320" spans="2:22" x14ac:dyDescent="0.3">
+    <row r="320" spans="2:29" x14ac:dyDescent="0.3">
       <c r="B320" s="38" t="str">
         <f>$D$305&amp;$E$305&amp;"2000"&amp;$G$305</f>
         <v>885000020002</v>
@@ -19222,17 +19863,17 @@
         <v>("885000030022","ปรับอากาศ","ตะแกรงแอร์");</v>
       </c>
     </row>
-    <row r="337" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="337" spans="1:30" x14ac:dyDescent="0.3">
       <c r="B337" s="31"/>
       <c r="C337" s="1"/>
       <c r="D337" s="1"/>
     </row>
-    <row r="338" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="338" spans="1:30" x14ac:dyDescent="0.3">
       <c r="B338" s="1"/>
       <c r="C338" s="1"/>
       <c r="D338" s="1"/>
     </row>
-    <row r="340" spans="1:22" ht="23.4" x14ac:dyDescent="0.45">
+    <row r="340" spans="1:30" ht="23.4" x14ac:dyDescent="0.45">
       <c r="B340" s="26" t="s">
         <v>440</v>
       </c>
@@ -19240,11 +19881,14 @@
         <f>"CREATE TABLE """ &amp;B340 &amp; """ ("</f>
         <v>CREATE TABLE "Deposite_TBL" (</v>
       </c>
-    </row>
-    <row r="341" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="AD340" t="s">
+        <v>724</v>
+      </c>
+    </row>
+    <row r="341" spans="1:30" x14ac:dyDescent="0.3">
       <c r="B341" s="5"/>
     </row>
-    <row r="342" spans="1:22" ht="18" x14ac:dyDescent="0.3">
+    <row r="342" spans="1:30" ht="18" x14ac:dyDescent="0.3">
       <c r="B342" s="22" t="s">
         <v>441</v>
       </c>
@@ -19264,8 +19908,11 @@
         <f>""""&amp;B342&amp;"""" &amp;"    "&amp; "INTEGER NOT NULL,"</f>
         <v>"DepositeID"    INTEGER NOT NULL,</v>
       </c>
-    </row>
-    <row r="343" spans="1:22" ht="18" x14ac:dyDescent="0.3">
+      <c r="AD342" t="s">
+        <v>725</v>
+      </c>
+    </row>
+    <row r="343" spans="1:30" ht="18" x14ac:dyDescent="0.3">
       <c r="B343" s="22"/>
       <c r="C343" s="23"/>
       <c r="D343" s="22"/>
@@ -19275,8 +19922,11 @@
         <f>""""&amp;C342&amp;"""" &amp;"    "&amp; "TEXT NOT NULL,"</f>
         <v>"Date"    TEXT NOT NULL,</v>
       </c>
-    </row>
-    <row r="344" spans="1:22" ht="18" x14ac:dyDescent="0.3">
+      <c r="AD343" t="s">
+        <v>726</v>
+      </c>
+    </row>
+    <row r="344" spans="1:30" ht="18" x14ac:dyDescent="0.3">
       <c r="B344" s="22"/>
       <c r="C344" s="23"/>
       <c r="D344" s="22"/>
@@ -19286,8 +19936,11 @@
         <f>""""&amp;D342&amp;"""" &amp;"    "&amp; "INTEGER NOT NULL,"</f>
         <v>"ItemBarcode"    INTEGER NOT NULL,</v>
       </c>
-    </row>
-    <row r="345" spans="1:22" ht="18" x14ac:dyDescent="0.3">
+      <c r="AD344" t="s">
+        <v>727</v>
+      </c>
+    </row>
+    <row r="345" spans="1:30" ht="18" x14ac:dyDescent="0.3">
       <c r="B345" s="22"/>
       <c r="C345" s="23"/>
       <c r="D345" s="22"/>
@@ -19297,8 +19950,11 @@
         <f>""""&amp;E342&amp;"""" &amp;"    "&amp; "INTEGER NOT NULL,"</f>
         <v>"Amount"    INTEGER NOT NULL,</v>
       </c>
-    </row>
-    <row r="346" spans="1:22" ht="18" x14ac:dyDescent="0.3">
+      <c r="AD345" t="s">
+        <v>728</v>
+      </c>
+    </row>
+    <row r="346" spans="1:30" ht="18" x14ac:dyDescent="0.3">
       <c r="B346" s="22"/>
       <c r="C346" s="23"/>
       <c r="D346" s="22"/>
@@ -19308,8 +19964,11 @@
         <f>""""&amp;F342&amp;"""" &amp;"    "&amp; "INTEGER NOT NULL,"</f>
         <v>"StaffID"    INTEGER NOT NULL,</v>
       </c>
-    </row>
-    <row r="347" spans="1:22" ht="18" x14ac:dyDescent="0.3">
+      <c r="AD346" t="s">
+        <v>729</v>
+      </c>
+    </row>
+    <row r="347" spans="1:30" ht="18" x14ac:dyDescent="0.3">
       <c r="B347" s="22"/>
       <c r="C347" s="23"/>
       <c r="D347" s="22"/>
@@ -19319,8 +19978,11 @@
         <f>"PRIMARY KEY("""&amp;  B342 &amp; """ AUTOINCREMENT)"</f>
         <v>PRIMARY KEY("DepositeID" AUTOINCREMENT)</v>
       </c>
-    </row>
-    <row r="348" spans="1:22" ht="18" x14ac:dyDescent="0.3">
+      <c r="AD347" t="s">
+        <v>730</v>
+      </c>
+    </row>
+    <row r="348" spans="1:30" ht="18" x14ac:dyDescent="0.3">
       <c r="B348" s="22"/>
       <c r="C348" s="23"/>
       <c r="D348" s="22"/>
@@ -19330,8 +19992,11 @@
         <f>"FOREIGN KEY("""&amp;D342&amp;""") " &amp; "REFERENCES """ &amp; B305&amp; """(""" &amp; B307 &amp;""")"</f>
         <v>FOREIGN KEY("ItemBarcode") REFERENCES "Asset_TBL"("Barcode")</v>
       </c>
-    </row>
-    <row r="349" spans="1:22" ht="18" x14ac:dyDescent="0.3">
+      <c r="AD348" t="s">
+        <v>731</v>
+      </c>
+    </row>
+    <row r="349" spans="1:30" ht="18" x14ac:dyDescent="0.3">
       <c r="B349" s="22"/>
       <c r="C349" s="23"/>
       <c r="D349" s="22"/>
@@ -19341,8 +20006,11 @@
         <f>"FOREIGN KEY("""&amp;F342&amp;""") " &amp; "REFERENCES """ &amp; B1&amp; """(""" &amp; B3 &amp;""")"</f>
         <v>FOREIGN KEY("StaffID") REFERENCES "Employee_TBL"("EmployeeID")</v>
       </c>
-    </row>
-    <row r="350" spans="1:22" ht="18" x14ac:dyDescent="0.3">
+      <c r="AD349" t="s">
+        <v>732</v>
+      </c>
+    </row>
+    <row r="350" spans="1:30" ht="18" x14ac:dyDescent="0.3">
       <c r="B350" s="22"/>
       <c r="C350" s="23"/>
       <c r="D350" s="22"/>
@@ -19351,8 +20019,11 @@
       <c r="V350" t="s">
         <v>518</v>
       </c>
-    </row>
-    <row r="351" spans="1:22" ht="18" x14ac:dyDescent="0.3">
+      <c r="AD350" t="s">
+        <v>695</v>
+      </c>
+    </row>
+    <row r="351" spans="1:30" ht="18" x14ac:dyDescent="0.3">
       <c r="B351" s="22"/>
       <c r="C351" s="23"/>
       <c r="D351" s="22"/>
@@ -19363,7 +20034,7 @@
         <v>INSERT INTO Deposite_TBL(Date,ItemBarcode,Amount,StaffID)</v>
       </c>
     </row>
-    <row r="352" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="352" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A352" t="s">
         <v>326</v>
       </c>
@@ -19754,7 +20425,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="369" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="369" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A369" t="s">
         <v>334</v>
       </c>
@@ -19774,7 +20445,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="370" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="370" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A370" t="s">
         <v>328</v>
       </c>
@@ -19794,7 +20465,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="371" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="371" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A371" t="s">
         <v>335</v>
       </c>
@@ -19814,7 +20485,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="372" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="372" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A372" t="s">
         <v>329</v>
       </c>
@@ -19834,56 +20505,56 @@
         <v>1</v>
       </c>
     </row>
-    <row r="373" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="373" spans="1:31" x14ac:dyDescent="0.3">
       <c r="B373" s="27"/>
       <c r="C373" s="27"/>
       <c r="D373" s="1"/>
       <c r="E373" s="10"/>
       <c r="F373" s="28"/>
     </row>
-    <row r="374" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="374" spans="1:31" x14ac:dyDescent="0.3">
       <c r="B374" s="10"/>
       <c r="C374" s="27"/>
       <c r="D374" s="10"/>
       <c r="E374" s="10"/>
       <c r="F374" s="10"/>
     </row>
-    <row r="375" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="375" spans="1:31" x14ac:dyDescent="0.3">
       <c r="B375" s="10"/>
       <c r="C375" s="27"/>
       <c r="D375" s="10"/>
       <c r="E375" s="10"/>
       <c r="F375" s="10"/>
     </row>
-    <row r="376" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="376" spans="1:31" x14ac:dyDescent="0.3">
       <c r="B376" s="10"/>
       <c r="C376" s="27"/>
       <c r="D376" s="10"/>
       <c r="E376" s="10"/>
       <c r="F376" s="10"/>
     </row>
-    <row r="377" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="377" spans="1:31" x14ac:dyDescent="0.3">
       <c r="B377" s="10"/>
       <c r="C377" s="27"/>
       <c r="D377" s="10"/>
       <c r="E377" s="10"/>
       <c r="F377" s="10"/>
     </row>
-    <row r="378" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="378" spans="1:31" x14ac:dyDescent="0.3">
       <c r="B378" s="10"/>
       <c r="C378" s="27"/>
       <c r="D378" s="10"/>
       <c r="E378" s="10"/>
       <c r="F378" s="10"/>
     </row>
-    <row r="379" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="379" spans="1:31" x14ac:dyDescent="0.3">
       <c r="B379" s="10"/>
       <c r="C379" s="10"/>
       <c r="D379" s="10"/>
       <c r="E379" s="10"/>
       <c r="F379" s="10"/>
     </row>
-    <row r="381" spans="1:22" ht="23.4" x14ac:dyDescent="0.45">
+    <row r="381" spans="1:31" ht="23.4" x14ac:dyDescent="0.45">
       <c r="B381" s="26" t="s">
         <v>439</v>
       </c>
@@ -19891,11 +20562,14 @@
         <f>"CREATE TABLE """ &amp;B381 &amp; """ ("</f>
         <v>CREATE TABLE "Withdraw_TBL" (</v>
       </c>
-    </row>
-    <row r="382" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="AE381" t="s">
+        <v>747</v>
+      </c>
+    </row>
+    <row r="382" spans="1:31" x14ac:dyDescent="0.3">
       <c r="B382" s="5"/>
     </row>
-    <row r="383" spans="1:22" ht="18" x14ac:dyDescent="0.3">
+    <row r="383" spans="1:31" ht="18" x14ac:dyDescent="0.3">
       <c r="B383" s="22" t="s">
         <v>442</v>
       </c>
@@ -19918,8 +20592,11 @@
         <f>""""&amp;B383&amp;"""" &amp;"    "&amp; "INTEGER NOT NULL,"</f>
         <v>"WithdrawID"    INTEGER NOT NULL,</v>
       </c>
-    </row>
-    <row r="384" spans="1:22" ht="18" x14ac:dyDescent="0.3">
+      <c r="AE383" t="s">
+        <v>748</v>
+      </c>
+    </row>
+    <row r="384" spans="1:31" ht="18" x14ac:dyDescent="0.3">
       <c r="B384" s="22"/>
       <c r="C384" s="23"/>
       <c r="D384" s="22"/>
@@ -19930,8 +20607,11 @@
         <f>""""&amp;C383&amp;"""" &amp;"    "&amp; "TEXT NOT NULL,"</f>
         <v>"Date"    TEXT NOT NULL,</v>
       </c>
-    </row>
-    <row r="385" spans="2:22" ht="18" x14ac:dyDescent="0.3">
+      <c r="AE384" t="s">
+        <v>726</v>
+      </c>
+    </row>
+    <row r="385" spans="2:31" ht="18" x14ac:dyDescent="0.3">
       <c r="B385" s="22"/>
       <c r="C385" s="23"/>
       <c r="D385" s="22"/>
@@ -19942,8 +20622,11 @@
         <f>""""&amp;D383&amp;"""" &amp;"    "&amp; "TEXT NOT NULL,"</f>
         <v>"ItemBarcode"    TEXT NOT NULL,</v>
       </c>
-    </row>
-    <row r="386" spans="2:22" ht="18" x14ac:dyDescent="0.3">
+      <c r="AE385" t="s">
+        <v>749</v>
+      </c>
+    </row>
+    <row r="386" spans="2:31" ht="18" x14ac:dyDescent="0.3">
       <c r="B386" s="22"/>
       <c r="C386" s="23"/>
       <c r="D386" s="22"/>
@@ -19954,8 +20637,11 @@
         <f>""""&amp;E383&amp;"""" &amp;"    "&amp; "INTEGER NOT NULL,"</f>
         <v>"Amount"    INTEGER NOT NULL,</v>
       </c>
-    </row>
-    <row r="387" spans="2:22" ht="18" x14ac:dyDescent="0.3">
+      <c r="AE386" t="s">
+        <v>728</v>
+      </c>
+    </row>
+    <row r="387" spans="2:31" ht="18" x14ac:dyDescent="0.3">
       <c r="B387" s="22"/>
       <c r="C387" s="23"/>
       <c r="D387" s="22"/>
@@ -19966,8 +20652,11 @@
         <f>""""&amp;F383&amp;"""" &amp;"    "&amp; "INTEGER NOT NULL,"</f>
         <v>"Withdrawer"    INTEGER NOT NULL,</v>
       </c>
-    </row>
-    <row r="388" spans="2:22" ht="18" x14ac:dyDescent="0.3">
+      <c r="AE387" t="s">
+        <v>750</v>
+      </c>
+    </row>
+    <row r="388" spans="2:31" ht="18" x14ac:dyDescent="0.3">
       <c r="B388" s="22"/>
       <c r="C388" s="23"/>
       <c r="D388" s="22"/>
@@ -19978,8 +20667,11 @@
         <f>""""&amp;G383&amp;"""" &amp;"    "&amp; "INTEGER NOT NULL,"</f>
         <v>"StaffID"    INTEGER NOT NULL,</v>
       </c>
-    </row>
-    <row r="389" spans="2:22" ht="18" x14ac:dyDescent="0.3">
+      <c r="AE388" t="s">
+        <v>729</v>
+      </c>
+    </row>
+    <row r="389" spans="2:31" ht="18" x14ac:dyDescent="0.3">
       <c r="B389" s="22"/>
       <c r="C389" s="23"/>
       <c r="D389" s="22"/>
@@ -19990,8 +20682,11 @@
         <f>"PRIMARY KEY("""&amp;  B383 &amp; """ AUTOINCREMENT)"</f>
         <v>PRIMARY KEY("WithdrawID" AUTOINCREMENT)</v>
       </c>
-    </row>
-    <row r="390" spans="2:22" ht="18" x14ac:dyDescent="0.3">
+      <c r="AE389" t="s">
+        <v>751</v>
+      </c>
+    </row>
+    <row r="390" spans="2:31" ht="18" x14ac:dyDescent="0.3">
       <c r="B390" s="22"/>
       <c r="C390" s="23"/>
       <c r="D390" s="22"/>
@@ -20002,8 +20697,11 @@
         <f>"FOREIGN KEY("""&amp;D383&amp;""") " &amp; "REFERENCES """ &amp; B305&amp; """(""" &amp; B307 &amp;""")"</f>
         <v>FOREIGN KEY("ItemBarcode") REFERENCES "Asset_TBL"("Barcode")</v>
       </c>
-    </row>
-    <row r="391" spans="2:22" ht="18" x14ac:dyDescent="0.3">
+      <c r="AE390" t="s">
+        <v>731</v>
+      </c>
+    </row>
+    <row r="391" spans="2:31" ht="18" x14ac:dyDescent="0.3">
       <c r="B391" s="22"/>
       <c r="C391" s="23"/>
       <c r="D391" s="22"/>
@@ -20014,8 +20712,11 @@
         <f>"FOREIGN KEY("""&amp;F383&amp;""") " &amp; "REFERENCES """ &amp; B27&amp; """(""" &amp; B29 &amp;""")"</f>
         <v>FOREIGN KEY("Withdrawer") REFERENCES "Customer_TBL"("CustomerID")</v>
       </c>
-    </row>
-    <row r="392" spans="2:22" ht="18" x14ac:dyDescent="0.3">
+      <c r="AE391" t="s">
+        <v>752</v>
+      </c>
+    </row>
+    <row r="392" spans="2:31" ht="18" x14ac:dyDescent="0.3">
       <c r="B392" s="22"/>
       <c r="C392" s="23"/>
       <c r="D392" s="22"/>
@@ -20026,8 +20727,11 @@
         <f>"FOREIGN KEY("""&amp;G383&amp;""") " &amp; "REFERENCES """ &amp; B1&amp; """(""" &amp; B3 &amp;""")"</f>
         <v>FOREIGN KEY("StaffID") REFERENCES "Employee_TBL"("EmployeeID")</v>
       </c>
-    </row>
-    <row r="393" spans="2:22" x14ac:dyDescent="0.3">
+      <c r="AE392" t="s">
+        <v>732</v>
+      </c>
+    </row>
+    <row r="393" spans="2:31" x14ac:dyDescent="0.3">
       <c r="B393" s="27">
         <v>1</v>
       </c>
@@ -20039,8 +20743,11 @@
       <c r="V393" t="s">
         <v>518</v>
       </c>
-    </row>
-    <row r="394" spans="2:22" x14ac:dyDescent="0.3">
+      <c r="AE393" t="s">
+        <v>695</v>
+      </c>
+    </row>
+    <row r="394" spans="2:31" x14ac:dyDescent="0.3">
       <c r="B394" s="27">
         <v>2</v>
       </c>
@@ -20050,7 +20757,7 @@
       <c r="F394" s="7"/>
       <c r="G394" s="28"/>
     </row>
-    <row r="395" spans="2:22" x14ac:dyDescent="0.3">
+    <row r="395" spans="2:31" x14ac:dyDescent="0.3">
       <c r="B395" s="27">
         <v>3</v>
       </c>
@@ -20060,7 +20767,7 @@
       <c r="F395" s="7"/>
       <c r="G395" s="28"/>
     </row>
-    <row r="396" spans="2:22" x14ac:dyDescent="0.3">
+    <row r="396" spans="2:31" x14ac:dyDescent="0.3">
       <c r="B396" s="27">
         <v>4</v>
       </c>
@@ -20070,7 +20777,7 @@
       <c r="F396" s="7"/>
       <c r="G396" s="28"/>
     </row>
-    <row r="397" spans="2:22" x14ac:dyDescent="0.3">
+    <row r="397" spans="2:31" x14ac:dyDescent="0.3">
       <c r="B397" s="27">
         <v>5</v>
       </c>
@@ -20080,7 +20787,7 @@
       <c r="F397" s="7"/>
       <c r="G397" s="28"/>
     </row>
-    <row r="398" spans="2:22" x14ac:dyDescent="0.3">
+    <row r="398" spans="2:31" x14ac:dyDescent="0.3">
       <c r="B398" s="27">
         <v>6</v>
       </c>
@@ -20090,7 +20797,7 @@
       <c r="F398" s="7"/>
       <c r="G398" s="28"/>
     </row>
-    <row r="399" spans="2:22" x14ac:dyDescent="0.3">
+    <row r="399" spans="2:31" x14ac:dyDescent="0.3">
       <c r="B399" s="27">
         <v>7</v>
       </c>
@@ -20100,7 +20807,7 @@
       <c r="F399" s="7"/>
       <c r="G399" s="28"/>
     </row>
-    <row r="400" spans="2:22" x14ac:dyDescent="0.3">
+    <row r="400" spans="2:31" x14ac:dyDescent="0.3">
       <c r="B400" s="27">
         <v>8</v>
       </c>
@@ -20110,7 +20817,7 @@
       <c r="F400" s="7"/>
       <c r="G400" s="28"/>
     </row>
-    <row r="401" spans="2:22" x14ac:dyDescent="0.3">
+    <row r="401" spans="2:33" x14ac:dyDescent="0.3">
       <c r="B401" s="27">
         <v>9</v>
       </c>
@@ -20120,7 +20827,7 @@
       <c r="F401" s="7"/>
       <c r="G401" s="28"/>
     </row>
-    <row r="402" spans="2:22" x14ac:dyDescent="0.3">
+    <row r="402" spans="2:33" x14ac:dyDescent="0.3">
       <c r="B402" s="27">
         <v>10</v>
       </c>
@@ -20130,7 +20837,7 @@
       <c r="F402" s="7"/>
       <c r="G402" s="28"/>
     </row>
-    <row r="403" spans="2:22" x14ac:dyDescent="0.3">
+    <row r="403" spans="2:33" x14ac:dyDescent="0.3">
       <c r="B403" s="27">
         <v>11</v>
       </c>
@@ -20140,7 +20847,7 @@
       <c r="F403" s="7"/>
       <c r="G403" s="28"/>
     </row>
-    <row r="404" spans="2:22" x14ac:dyDescent="0.3">
+    <row r="404" spans="2:33" x14ac:dyDescent="0.3">
       <c r="B404" s="27">
         <v>12</v>
       </c>
@@ -20150,7 +20857,7 @@
       <c r="F404" s="7"/>
       <c r="G404" s="28"/>
     </row>
-    <row r="405" spans="2:22" x14ac:dyDescent="0.3">
+    <row r="405" spans="2:33" x14ac:dyDescent="0.3">
       <c r="B405" s="10"/>
       <c r="C405" s="31"/>
       <c r="D405" s="1"/>
@@ -20158,7 +20865,7 @@
       <c r="F405" s="7"/>
       <c r="G405" s="10"/>
     </row>
-    <row r="406" spans="2:22" x14ac:dyDescent="0.3">
+    <row r="406" spans="2:33" x14ac:dyDescent="0.3">
       <c r="B406" s="10"/>
       <c r="C406" s="31"/>
       <c r="D406" s="1"/>
@@ -20166,7 +20873,7 @@
       <c r="F406" s="7"/>
       <c r="G406" s="10"/>
     </row>
-    <row r="407" spans="2:22" x14ac:dyDescent="0.3">
+    <row r="407" spans="2:33" x14ac:dyDescent="0.3">
       <c r="B407" s="10"/>
       <c r="C407" s="31"/>
       <c r="D407" s="1"/>
@@ -20174,7 +20881,7 @@
       <c r="F407" s="1"/>
       <c r="G407" s="10"/>
     </row>
-    <row r="408" spans="2:22" x14ac:dyDescent="0.3">
+    <row r="408" spans="2:33" x14ac:dyDescent="0.3">
       <c r="B408" s="10"/>
       <c r="C408" s="31"/>
       <c r="D408" s="1"/>
@@ -20182,7 +20889,7 @@
       <c r="F408" s="1"/>
       <c r="G408" s="10"/>
     </row>
-    <row r="409" spans="2:22" x14ac:dyDescent="0.3">
+    <row r="409" spans="2:33" x14ac:dyDescent="0.3">
       <c r="B409" s="10"/>
       <c r="C409" s="31"/>
       <c r="D409" s="1"/>
@@ -20190,7 +20897,7 @@
       <c r="F409" s="1"/>
       <c r="G409" s="10"/>
     </row>
-    <row r="410" spans="2:22" x14ac:dyDescent="0.3">
+    <row r="410" spans="2:33" x14ac:dyDescent="0.3">
       <c r="B410" s="10"/>
       <c r="C410" s="1"/>
       <c r="D410" s="1"/>
@@ -20198,7 +20905,7 @@
       <c r="F410" s="1"/>
       <c r="G410" s="10"/>
     </row>
-    <row r="415" spans="2:22" ht="23.4" x14ac:dyDescent="0.45">
+    <row r="415" spans="2:33" ht="23.4" x14ac:dyDescent="0.45">
       <c r="B415" s="26" t="s">
         <v>686</v>
       </c>
@@ -20210,11 +20917,20 @@
         <f>"CREATE TABLE """ &amp;B415 &amp; """ ("</f>
         <v>CREATE TABLE "Access_Card_Manage_TBL" (</v>
       </c>
-    </row>
-    <row r="416" spans="2:22" x14ac:dyDescent="0.3">
+      <c r="AE415" t="s">
+        <v>687</v>
+      </c>
+    </row>
+    <row r="416" spans="2:33" x14ac:dyDescent="0.3">
       <c r="B416" s="5"/>
-    </row>
-    <row r="417" spans="1:22" ht="18" x14ac:dyDescent="0.3">
+      <c r="AF416" t="s">
+        <v>617</v>
+      </c>
+      <c r="AG416" t="s">
+        <v>688</v>
+      </c>
+    </row>
+    <row r="417" spans="1:33" ht="18" x14ac:dyDescent="0.3">
       <c r="B417" s="22" t="s">
         <v>617</v>
       </c>
@@ -20234,8 +20950,14 @@
         <f>""""&amp;B417&amp;"""" &amp;"    "&amp; "INTEGER NOT NULL,"</f>
         <v>"ID"    INTEGER NOT NULL,</v>
       </c>
-    </row>
-    <row r="418" spans="1:22" ht="18" x14ac:dyDescent="0.3">
+      <c r="AF417" t="s">
+        <v>689</v>
+      </c>
+      <c r="AG417" t="s">
+        <v>690</v>
+      </c>
+    </row>
+    <row r="418" spans="1:33" ht="18" x14ac:dyDescent="0.3">
       <c r="B418" s="22"/>
       <c r="C418" s="22"/>
       <c r="D418" s="22"/>
@@ -20245,8 +20967,14 @@
         <f>""""&amp;C417&amp;"""" &amp;"    "&amp; "INTEGER NOT NULL,"</f>
         <v>"KeycardID"    INTEGER NOT NULL,</v>
       </c>
-    </row>
-    <row r="419" spans="1:22" ht="18" x14ac:dyDescent="0.3">
+      <c r="AF418" t="s">
+        <v>552</v>
+      </c>
+      <c r="AG418" t="s">
+        <v>688</v>
+      </c>
+    </row>
+    <row r="419" spans="1:33" ht="18" x14ac:dyDescent="0.3">
       <c r="B419" s="22"/>
       <c r="C419" s="22"/>
       <c r="D419" s="22"/>
@@ -20256,8 +20984,14 @@
         <f>""""&amp;D417&amp;"""" &amp;"    "&amp; "INTEGER,"</f>
         <v>"CustomerID"    INTEGER,</v>
       </c>
-    </row>
-    <row r="420" spans="1:22" ht="18" x14ac:dyDescent="0.3">
+      <c r="AF419" t="s">
+        <v>407</v>
+      </c>
+      <c r="AG419" t="s">
+        <v>691</v>
+      </c>
+    </row>
+    <row r="420" spans="1:33" ht="18" x14ac:dyDescent="0.3">
       <c r="B420" s="22"/>
       <c r="C420" s="22"/>
       <c r="D420" s="22"/>
@@ -20267,8 +21001,15 @@
         <f>""""&amp;E417&amp;"""" &amp;"    "&amp; "INTEGER NOT NULL,"</f>
         <v>"StaffID"    INTEGER NOT NULL,</v>
       </c>
-    </row>
-    <row r="421" spans="1:22" ht="18" x14ac:dyDescent="0.3">
+      <c r="AF420" t="s">
+        <v>522</v>
+      </c>
+      <c r="AG420" t="s">
+        <v>691</v>
+      </c>
+    </row>
+    <row r="421" spans="1:33" ht="18" x14ac:dyDescent="0.3">
+      <c r="A421" s="53"/>
       <c r="B421" s="22"/>
       <c r="C421" s="22"/>
       <c r="D421" s="22"/>
@@ -20278,8 +21019,14 @@
         <f>""""&amp;F417&amp;"""" &amp;"    "&amp; "TEXT NOT NULL,"</f>
         <v>"Status"    TEXT NOT NULL,</v>
       </c>
-    </row>
-    <row r="422" spans="1:22" ht="18" x14ac:dyDescent="0.3">
+      <c r="AF421" t="s">
+        <v>416</v>
+      </c>
+      <c r="AG421" t="s">
+        <v>690</v>
+      </c>
+    </row>
+    <row r="422" spans="1:33" ht="18" x14ac:dyDescent="0.3">
       <c r="B422" s="22"/>
       <c r="C422" s="22"/>
       <c r="D422" s="22"/>
@@ -20289,8 +21036,11 @@
         <f>"PRIMARY KEY("""&amp;  B417 &amp; """ )"</f>
         <v>PRIMARY KEY("ID" )</v>
       </c>
-    </row>
-    <row r="423" spans="1:22" ht="18" x14ac:dyDescent="0.3">
+      <c r="AF422" t="s">
+        <v>692</v>
+      </c>
+    </row>
+    <row r="423" spans="1:33" ht="18" x14ac:dyDescent="0.3">
       <c r="A423" s="59" t="s">
         <v>138</v>
       </c>
@@ -20310,8 +21060,11 @@
         <f>"FOREIGN KEY("""&amp;D417&amp;""") " &amp; "REFERENCES """ &amp; B27&amp; """(""" &amp; B29 &amp;""")"</f>
         <v>FOREIGN KEY("CustomerID") REFERENCES "Customer_TBL"("CustomerID")</v>
       </c>
-    </row>
-    <row r="424" spans="1:22" ht="18" x14ac:dyDescent="0.3">
+      <c r="AF423" t="s">
+        <v>693</v>
+      </c>
+    </row>
+    <row r="424" spans="1:33" ht="18" x14ac:dyDescent="0.3">
       <c r="A424" s="59" t="s">
         <v>139</v>
       </c>
@@ -20331,8 +21084,11 @@
         <f>"FOREIGN KEY("""&amp;E417&amp;""") " &amp; "REFERENCES """ &amp; B1&amp; """(""" &amp; B3 &amp;""")"</f>
         <v>FOREIGN KEY("StaffID") REFERENCES "Employee_TBL"("EmployeeID")</v>
       </c>
-    </row>
-    <row r="425" spans="1:22" ht="18" x14ac:dyDescent="0.3">
+      <c r="AF424" t="s">
+        <v>694</v>
+      </c>
+    </row>
+    <row r="425" spans="1:33" ht="18" x14ac:dyDescent="0.3">
       <c r="A425" s="59" t="s">
         <v>140</v>
       </c>
@@ -20351,8 +21107,11 @@
       <c r="V425" t="s">
         <v>518</v>
       </c>
-    </row>
-    <row r="426" spans="1:22" ht="18" x14ac:dyDescent="0.3">
+      <c r="AE425" t="s">
+        <v>695</v>
+      </c>
+    </row>
+    <row r="426" spans="1:33" ht="18" x14ac:dyDescent="0.3">
       <c r="A426" s="59" t="s">
         <v>141</v>
       </c>
@@ -20369,7 +21128,7 @@
         <v>685</v>
       </c>
     </row>
-    <row r="427" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="427" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A427" s="59" t="s">
         <v>142</v>
       </c>
@@ -20386,7 +21145,7 @@
         <v>685</v>
       </c>
     </row>
-    <row r="428" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="428" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A428" s="59" t="s">
         <v>143</v>
       </c>
@@ -20407,7 +21166,7 @@
         <v>INSERT INTO Access_Card_Manage_TBL(KeycardID)</v>
       </c>
     </row>
-    <row r="429" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="429" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A429" s="59" t="s">
         <v>144</v>
       </c>
@@ -20431,7 +21190,7 @@
         <v>("885000000002001"),</v>
       </c>
     </row>
-    <row r="430" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="430" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A430" s="59" t="s">
         <v>145</v>
       </c>
@@ -20452,7 +21211,7 @@
         <v>("885000000002002"),</v>
       </c>
     </row>
-    <row r="431" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="431" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A431" s="59" t="s">
         <v>146</v>
       </c>
@@ -20473,7 +21232,7 @@
         <v>("885000000002003"),</v>
       </c>
     </row>
-    <row r="432" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="432" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A432" s="59" t="s">
         <v>147</v>
       </c>
@@ -22425,7 +23184,7 @@
       <c r="E525" s="1"/>
       <c r="F525" s="1"/>
       <c r="V525" t="str">
-        <f t="shared" ref="V525:V556" si="11">"("&amp;FunNoo&amp;C519&amp;"""),"</f>
+        <f t="shared" ref="V525:V528" si="11">"("&amp;FunNoo&amp;C519&amp;"""),"</f>
         <v>("885000000002097"),</v>
       </c>
     </row>
@@ -22712,7 +23471,7 @@
       <c r="E559" s="1"/>
       <c r="F559" s="1"/>
     </row>
-    <row r="562" spans="2:22" ht="23.4" x14ac:dyDescent="0.45">
+    <row r="562" spans="2:31" ht="23.4" x14ac:dyDescent="0.45">
       <c r="B562" s="26" t="s">
         <v>557</v>
       </c>
@@ -22721,11 +23480,20 @@
         <f>"CREATE TABLE """ &amp;B562 &amp; """ ("</f>
         <v>CREATE TABLE "Interested_People_TBL" (</v>
       </c>
-    </row>
-    <row r="563" spans="2:22" x14ac:dyDescent="0.3">
+      <c r="AC562" t="s">
+        <v>742</v>
+      </c>
+    </row>
+    <row r="563" spans="2:31" x14ac:dyDescent="0.3">
       <c r="B563" s="5"/>
-    </row>
-    <row r="564" spans="2:22" ht="18" x14ac:dyDescent="0.3">
+      <c r="AD563" t="s">
+        <v>558</v>
+      </c>
+      <c r="AE563" t="s">
+        <v>688</v>
+      </c>
+    </row>
+    <row r="564" spans="2:31" ht="18" x14ac:dyDescent="0.3">
       <c r="B564" s="22" t="s">
         <v>558</v>
       </c>
@@ -22748,8 +23516,14 @@
         <f>""""&amp;B565&amp;"""" &amp;"    "&amp; "INTEGER NOT NULL,"</f>
         <v>""    INTEGER NOT NULL,</v>
       </c>
-    </row>
-    <row r="565" spans="2:22" ht="18" x14ac:dyDescent="0.3">
+      <c r="AD564" t="s">
+        <v>425</v>
+      </c>
+      <c r="AE564" t="s">
+        <v>710</v>
+      </c>
+    </row>
+    <row r="565" spans="2:31" ht="18" x14ac:dyDescent="0.3">
       <c r="B565" s="22"/>
       <c r="C565" s="56" t="s">
         <v>627</v>
@@ -22770,8 +23544,14 @@
         <f>""""&amp;C565&amp;"""" &amp;"    "&amp; "TEXT NOT NULL,"</f>
         <v>"10/8/2023"    TEXT NOT NULL,</v>
       </c>
-    </row>
-    <row r="566" spans="2:22" ht="18" x14ac:dyDescent="0.3">
+      <c r="AD565" t="s">
+        <v>402</v>
+      </c>
+      <c r="AE565" t="s">
+        <v>690</v>
+      </c>
+    </row>
+    <row r="566" spans="2:31" ht="18" x14ac:dyDescent="0.3">
       <c r="B566" s="22"/>
       <c r="C566" s="56" t="s">
         <v>627</v>
@@ -22792,8 +23572,14 @@
         <f>""""&amp;D565&amp;"""" &amp;"    "&amp; "TEXT NOT NULL,"</f>
         <v>"pim"    TEXT NOT NULL,</v>
       </c>
-    </row>
-    <row r="567" spans="2:22" ht="18" x14ac:dyDescent="0.3">
+      <c r="AD566" t="s">
+        <v>559</v>
+      </c>
+      <c r="AE566" t="s">
+        <v>690</v>
+      </c>
+    </row>
+    <row r="567" spans="2:31" ht="18" x14ac:dyDescent="0.3">
       <c r="B567" s="22"/>
       <c r="C567" s="56" t="s">
         <v>627</v>
@@ -22814,8 +23600,14 @@
         <f>""""&amp;E565&amp;"""" &amp;"    "&amp; "TEXT NOT NULL,"</f>
         <v>"081-2576569"    TEXT NOT NULL,</v>
       </c>
-    </row>
-    <row r="568" spans="2:22" ht="18" x14ac:dyDescent="0.3">
+      <c r="AD567" t="s">
+        <v>411</v>
+      </c>
+      <c r="AE567" t="s">
+        <v>690</v>
+      </c>
+    </row>
+    <row r="568" spans="2:31" ht="18" x14ac:dyDescent="0.3">
       <c r="B568" s="22"/>
       <c r="C568" s="56" t="s">
         <v>627</v>
@@ -22836,8 +23628,14 @@
         <f>""""&amp;F565&amp;"""" &amp;"    "&amp; "TEXT NOT NULL,"</f>
         <v>"pimLine"    TEXT NOT NULL,</v>
       </c>
-    </row>
-    <row r="569" spans="2:22" ht="18" x14ac:dyDescent="0.3">
+      <c r="AD568" t="s">
+        <v>577</v>
+      </c>
+      <c r="AE568" t="s">
+        <v>690</v>
+      </c>
+    </row>
+    <row r="569" spans="2:31" ht="18" x14ac:dyDescent="0.3">
       <c r="B569" s="22"/>
       <c r="C569" s="56" t="s">
         <v>627</v>
@@ -22858,14 +23656,20 @@
         <f>""""&amp;G565&amp;"""" &amp;"    "&amp; "TEXT NOT NULL,"</f>
         <v>"-"    TEXT NOT NULL,</v>
       </c>
-    </row>
-    <row r="570" spans="2:22" x14ac:dyDescent="0.3">
+      <c r="AD569" t="s">
+        <v>743</v>
+      </c>
+    </row>
+    <row r="570" spans="2:31" x14ac:dyDescent="0.3">
       <c r="V570" t="str">
         <f>"PRIMARY KEY("""&amp;  B565 &amp; """ )"</f>
         <v>PRIMARY KEY("" )</v>
       </c>
-    </row>
-    <row r="571" spans="2:22" x14ac:dyDescent="0.3">
+      <c r="AC570" t="s">
+        <v>695</v>
+      </c>
+    </row>
+    <row r="571" spans="2:31" x14ac:dyDescent="0.3">
       <c r="V571" t="s">
         <v>518</v>
       </c>
@@ -22945,10 +23749,78 @@
         <v>("","","","",""),</v>
       </c>
     </row>
-    <row r="593" spans="22:22" x14ac:dyDescent="0.3">
+    <row r="593" spans="22:24" x14ac:dyDescent="0.3">
       <c r="V593" t="str">
         <f>"("&amp;FunNoo&amp;C593&amp;FunNooComma&amp;FunNoo&amp;D593&amp;FunNooComma&amp;FunNoo&amp;E593&amp;FunNooComma&amp;FunNoo&amp;F593&amp;FunNooComma&amp;FunNoo&amp;G593&amp;""");"</f>
         <v>("","","","","");</v>
+      </c>
+    </row>
+    <row r="605" spans="22:24" x14ac:dyDescent="0.3">
+      <c r="V605" t="s">
+        <v>715</v>
+      </c>
+    </row>
+    <row r="606" spans="22:24" x14ac:dyDescent="0.3">
+      <c r="W606" t="s">
+        <v>630</v>
+      </c>
+      <c r="X606" t="s">
+        <v>688</v>
+      </c>
+    </row>
+    <row r="607" spans="22:24" x14ac:dyDescent="0.3">
+      <c r="W607" t="s">
+        <v>716</v>
+      </c>
+      <c r="X607" t="s">
+        <v>710</v>
+      </c>
+    </row>
+    <row r="608" spans="22:24" x14ac:dyDescent="0.3">
+      <c r="W608" t="s">
+        <v>415</v>
+      </c>
+      <c r="X608" t="s">
+        <v>710</v>
+      </c>
+    </row>
+    <row r="609" spans="22:24" x14ac:dyDescent="0.3">
+      <c r="W609" t="s">
+        <v>616</v>
+      </c>
+      <c r="X609" t="s">
+        <v>717</v>
+      </c>
+    </row>
+    <row r="610" spans="22:24" x14ac:dyDescent="0.3">
+      <c r="W610" t="s">
+        <v>407</v>
+      </c>
+      <c r="X610" t="s">
+        <v>688</v>
+      </c>
+    </row>
+    <row r="611" spans="22:24" x14ac:dyDescent="0.3">
+      <c r="W611" t="s">
+        <v>414</v>
+      </c>
+      <c r="X611" t="s">
+        <v>718</v>
+      </c>
+    </row>
+    <row r="612" spans="22:24" x14ac:dyDescent="0.3">
+      <c r="W612" t="s">
+        <v>719</v>
+      </c>
+    </row>
+    <row r="613" spans="22:24" x14ac:dyDescent="0.3">
+      <c r="W613" t="s">
+        <v>714</v>
+      </c>
+    </row>
+    <row r="614" spans="22:24" x14ac:dyDescent="0.3">
+      <c r="V614" t="s">
+        <v>695</v>
       </c>
     </row>
   </sheetData>
@@ -22964,7 +23836,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{67562A3C-C307-447D-B66D-4E567D9DE81F}">
   <dimension ref="P4"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="Q12" sqref="Q12"/>
     </sheetView>
   </sheetViews>

</xml_diff>